<commit_message>
New files regarding clonal traits and storage + final trait data table
</commit_message>
<xml_diff>
--- a/Files/Trait data.xlsx
+++ b/Files/Trait data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PhD\Travels\Bilbao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PhD\Travels\Euskal_fd\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8055A543-2FE7-4B08-92FE-45AE17741AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD8F8DB-E97B-42B1-8085-9E8D69E4F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9456" yWindow="0" windowWidth="13584" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trait table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="427">
   <si>
     <t>Genus</t>
   </si>
@@ -1042,6 +1042,282 @@
   </si>
   <si>
     <t>D078</t>
+  </si>
+  <si>
+    <t>montana</t>
+  </si>
+  <si>
+    <t>08.05.</t>
+  </si>
+  <si>
+    <t>ARAN2</t>
+  </si>
+  <si>
+    <t>F003</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>F005</t>
+  </si>
+  <si>
+    <t>F006</t>
+  </si>
+  <si>
+    <t>F007</t>
+  </si>
+  <si>
+    <t>F008</t>
+  </si>
+  <si>
+    <t>F009</t>
+  </si>
+  <si>
+    <t>F010</t>
+  </si>
+  <si>
+    <t>F011</t>
+  </si>
+  <si>
+    <t>F012</t>
+  </si>
+  <si>
+    <t>09.05.</t>
+  </si>
+  <si>
+    <t>UR1</t>
+  </si>
+  <si>
+    <t>G057</t>
+  </si>
+  <si>
+    <t>G058</t>
+  </si>
+  <si>
+    <t>G059</t>
+  </si>
+  <si>
+    <t>G060</t>
+  </si>
+  <si>
+    <t>G061</t>
+  </si>
+  <si>
+    <t>G062</t>
+  </si>
+  <si>
+    <t>UR1&amp;2</t>
+  </si>
+  <si>
+    <t>G017</t>
+  </si>
+  <si>
+    <t>G018</t>
+  </si>
+  <si>
+    <t>G019</t>
+  </si>
+  <si>
+    <t>G020</t>
+  </si>
+  <si>
+    <t>G021</t>
+  </si>
+  <si>
+    <t>G022</t>
+  </si>
+  <si>
+    <t>G023</t>
+  </si>
+  <si>
+    <t>F001</t>
+  </si>
+  <si>
+    <t>F002</t>
+  </si>
+  <si>
+    <t>Hypericum</t>
+  </si>
+  <si>
+    <t>hirsutum</t>
+  </si>
+  <si>
+    <t>UR2</t>
+  </si>
+  <si>
+    <t>G011</t>
+  </si>
+  <si>
+    <t>G012</t>
+  </si>
+  <si>
+    <t>G013</t>
+  </si>
+  <si>
+    <t>G014</t>
+  </si>
+  <si>
+    <t>G015</t>
+  </si>
+  <si>
+    <t>G016</t>
+  </si>
+  <si>
+    <t>G063</t>
+  </si>
+  <si>
+    <t>G064</t>
+  </si>
+  <si>
+    <t>G065</t>
+  </si>
+  <si>
+    <t>G001</t>
+  </si>
+  <si>
+    <t>G002</t>
+  </si>
+  <si>
+    <t>G003</t>
+  </si>
+  <si>
+    <t>G004</t>
+  </si>
+  <si>
+    <t>G005</t>
+  </si>
+  <si>
+    <t>Carex</t>
+  </si>
+  <si>
+    <t>flacca</t>
+  </si>
+  <si>
+    <t>G006</t>
+  </si>
+  <si>
+    <t>G007</t>
+  </si>
+  <si>
+    <t>G008</t>
+  </si>
+  <si>
+    <t>G009</t>
+  </si>
+  <si>
+    <t>G010</t>
+  </si>
+  <si>
+    <t>G037</t>
+  </si>
+  <si>
+    <t>G038</t>
+  </si>
+  <si>
+    <t>G039</t>
+  </si>
+  <si>
+    <t>G040</t>
+  </si>
+  <si>
+    <t>G041</t>
+  </si>
+  <si>
+    <t>G042</t>
+  </si>
+  <si>
+    <t>Rubia</t>
+  </si>
+  <si>
+    <t>peregrina</t>
+  </si>
+  <si>
+    <t>G024</t>
+  </si>
+  <si>
+    <t>G025</t>
+  </si>
+  <si>
+    <t>G026</t>
+  </si>
+  <si>
+    <t>G027</t>
+  </si>
+  <si>
+    <t>G028</t>
+  </si>
+  <si>
+    <t>G029</t>
+  </si>
+  <si>
+    <t>G030</t>
+  </si>
+  <si>
+    <t>G031</t>
+  </si>
+  <si>
+    <t>G032</t>
+  </si>
+  <si>
+    <t>G033</t>
+  </si>
+  <si>
+    <t>G034</t>
+  </si>
+  <si>
+    <t>G035</t>
+  </si>
+  <si>
+    <t>G036</t>
+  </si>
+  <si>
+    <t>Sanicula</t>
+  </si>
+  <si>
+    <t>europaea</t>
+  </si>
+  <si>
+    <t>G043</t>
+  </si>
+  <si>
+    <t>G046</t>
+  </si>
+  <si>
+    <t>G045</t>
+  </si>
+  <si>
+    <t>G047</t>
+  </si>
+  <si>
+    <t>xylosteum</t>
+  </si>
+  <si>
+    <t>G048</t>
+  </si>
+  <si>
+    <t>G049</t>
+  </si>
+  <si>
+    <t>G050</t>
+  </si>
+  <si>
+    <t>G051</t>
+  </si>
+  <si>
+    <t>G052</t>
+  </si>
+  <si>
+    <t>G053</t>
+  </si>
+  <si>
+    <t>G054</t>
+  </si>
+  <si>
+    <t>G055</t>
+  </si>
+  <si>
+    <t>G056</t>
   </si>
 </sst>
 </file>
@@ -1402,11 +1678,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M217"/>
+  <dimension ref="A1:M291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L202" sqref="L202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1524,7 +1800,7 @@
         <v>0.23499999999999999</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K66" si="0">I3/G3</f>
+        <f>I3/G3</f>
         <v>0.12252346193952034</v>
       </c>
       <c r="M3">
@@ -1560,7 +1836,7 @@
         <v>0.04</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f>I4/G4</f>
         <v>0.14869888475836432</v>
       </c>
       <c r="M4">
@@ -1596,7 +1872,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f>I5/G5</f>
         <v>0.16058394160583939</v>
       </c>
       <c r="M5">
@@ -1632,7 +1908,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f>I6/G6</f>
         <v>0.1404494382022472</v>
       </c>
       <c r="M6">
@@ -1668,7 +1944,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f>I7/G7</f>
         <v>0.15617715617715619</v>
       </c>
       <c r="M7">
@@ -1704,7 +1980,7 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f>I8/G8</f>
         <v>8.5558931712777869E-2</v>
       </c>
       <c r="M8">
@@ -1740,7 +2016,7 @@
         <v>0.376</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
+        <f>I9/G9</f>
         <v>0.39788359788359789</v>
       </c>
       <c r="M9">
@@ -1776,7 +2052,7 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
+        <f>I10/G10</f>
         <v>0.41915227629513346</v>
       </c>
       <c r="M10">
@@ -1812,7 +2088,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f>I11/G11</f>
         <v>0.27756653992395436</v>
       </c>
       <c r="M11">
@@ -1848,7 +2124,7 @@
         <v>6.3E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f>I12/G12</f>
         <v>0.24230769230769231</v>
       </c>
       <c r="M12">
@@ -1884,7 +2160,7 @@
         <v>6.3E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f>I13/G13</f>
         <v>0.21501706484641639</v>
       </c>
       <c r="M13">
@@ -1920,7 +2196,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f>I14/G14</f>
         <v>0.22950819672131148</v>
       </c>
       <c r="M14">
@@ -1956,7 +2232,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f>I15/G15</f>
         <v>0.25925925925925924</v>
       </c>
       <c r="M15">
@@ -1992,7 +2268,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
+        <f>I16/G16</f>
         <v>0.21739130434782608</v>
       </c>
       <c r="M16">
@@ -2028,7 +2304,7 @@
         <v>0.47599999999999998</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
+        <f>I17/G17</f>
         <v>0.25925925925925924</v>
       </c>
       <c r="M17">
@@ -2064,7 +2340,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
+        <f>I18/G18</f>
         <v>0.27569331158238175</v>
       </c>
       <c r="M18">
@@ -2100,7 +2376,7 @@
         <v>0.36699999999999999</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
+        <f>I19/G19</f>
         <v>0.25051194539249144</v>
       </c>
       <c r="M19">
@@ -2136,7 +2412,7 @@
         <v>0.189</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
+        <f>I20/G20</f>
         <v>0.29032258064516125</v>
       </c>
       <c r="M20">
@@ -2172,7 +2448,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
+        <f>I21/G21</f>
         <v>0.21188630490956073</v>
       </c>
       <c r="M21">
@@ -2208,7 +2484,7 @@
         <v>0.124</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
+        <f>I22/G22</f>
         <v>0.40522875816993464</v>
       </c>
       <c r="M22">
@@ -2244,7 +2520,7 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
+        <f>I23/G23</f>
         <v>0.17229129662522205</v>
       </c>
       <c r="M23">
@@ -2280,7 +2556,7 @@
         <v>0.24</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
+        <f>I24/G24</f>
         <v>0.13392857142857142</v>
       </c>
       <c r="M24">
@@ -2316,7 +2592,7 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
+        <f>I25/G25</f>
         <v>0.15053091817613992</v>
       </c>
       <c r="M25">
@@ -2352,7 +2628,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
+        <f>I26/G26</f>
         <v>0.34635416666666669</v>
       </c>
       <c r="M26">
@@ -2388,7 +2664,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
+        <f>I27/G27</f>
         <v>0.36818181818181817</v>
       </c>
       <c r="M27">
@@ -2424,7 +2700,7 @@
         <v>0.111</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
+        <f>I28/G28</f>
         <v>0.36513157894736842</v>
       </c>
       <c r="M28">
@@ -2460,7 +2736,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
+        <f>I29/G29</f>
         <v>0.10144927536231883</v>
       </c>
       <c r="M29">
@@ -2496,7 +2772,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
+        <f>I30/G30</f>
         <v>0.16760828625235402</v>
       </c>
       <c r="M30">
@@ -2532,7 +2808,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
+        <f>I31/G31</f>
         <v>0.15594855305466238</v>
       </c>
       <c r="M31">
@@ -2568,7 +2844,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
+        <f>I32/G32</f>
         <v>0.13809523809523808</v>
       </c>
       <c r="M32">
@@ -2604,7 +2880,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
+        <f>I33/G33</f>
         <v>0.2299465240641711</v>
       </c>
       <c r="M33">
@@ -2640,7 +2916,7 @@
         <v>0.186</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
+        <f>I34/G34</f>
         <v>0.25340599455040874</v>
       </c>
       <c r="M34">
@@ -2676,7 +2952,7 @@
         <v>0.155</v>
       </c>
       <c r="K35">
-        <f t="shared" si="0"/>
+        <f>I35/G35</f>
         <v>0.22794117647058823</v>
       </c>
       <c r="M35">
@@ -2712,7 +2988,7 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="K36">
-        <f t="shared" si="0"/>
+        <f>I36/G36</f>
         <v>0.26106526631657911</v>
       </c>
       <c r="M36">
@@ -2748,7 +3024,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
+        <f>I37/G37</f>
         <v>0.11817726589884826</v>
       </c>
       <c r="M37">
@@ -2784,7 +3060,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
+        <f>I38/G38</f>
         <v>0.18032786885245902</v>
       </c>
       <c r="M38">
@@ -2820,7 +3096,7 @@
         <v>0.27300000000000002</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
+        <f>I39/G39</f>
         <v>0.2426666666666667</v>
       </c>
       <c r="M39">
@@ -2856,7 +3132,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
+        <f>I40/G40</f>
         <v>0.13983050847457629</v>
       </c>
       <c r="M40">
@@ -2889,7 +3165,7 @@
         <v>0.05</v>
       </c>
       <c r="K41">
-        <f t="shared" si="0"/>
+        <f>I41/G41</f>
         <v>0.43859649122807021</v>
       </c>
       <c r="L41" t="s">
@@ -2928,7 +3204,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K42">
-        <f t="shared" si="0"/>
+        <f>I42/G42</f>
         <v>0.125</v>
       </c>
       <c r="M42">
@@ -2964,7 +3240,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" si="0"/>
+        <f>I43/G43</f>
         <v>0.33500000000000002</v>
       </c>
       <c r="M43">
@@ -3000,7 +3276,7 @@
         <v>0.128</v>
       </c>
       <c r="K44">
-        <f t="shared" si="0"/>
+        <f>I44/G44</f>
         <v>0.32569974554707376</v>
       </c>
       <c r="M44">
@@ -3036,7 +3312,7 @@
         <v>0.66800000000000004</v>
       </c>
       <c r="K45">
-        <f t="shared" si="0"/>
+        <f>I45/G45</f>
         <v>7.6030047803323481E-2</v>
       </c>
       <c r="M45">
@@ -3072,7 +3348,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K46">
-        <f t="shared" si="0"/>
+        <f>I46/G46</f>
         <v>7.5952693823915896E-2</v>
       </c>
       <c r="M46">
@@ -3108,7 +3384,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K47">
-        <f t="shared" si="0"/>
+        <f>I47/G47</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="M47">
@@ -3144,7 +3420,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K48">
-        <f t="shared" si="0"/>
+        <f>I48/G48</f>
         <v>0.17156862745098037</v>
       </c>
       <c r="M48">
@@ -3180,7 +3456,7 @@
         <v>0.224</v>
       </c>
       <c r="K49">
-        <f t="shared" si="0"/>
+        <f>I49/G49</f>
         <v>0.15774647887323945</v>
       </c>
       <c r="M49">
@@ -3216,7 +3492,7 @@
         <v>0.36799999999999999</v>
       </c>
       <c r="K50">
-        <f t="shared" si="0"/>
+        <f>I50/G50</f>
         <v>0.16211453744493393</v>
       </c>
       <c r="M50">
@@ -3255,7 +3531,7 @@
         <v>104</v>
       </c>
       <c r="K51">
-        <f t="shared" si="0"/>
+        <f>I51/G51</f>
         <v>0.18175338560228083</v>
       </c>
       <c r="M51">
@@ -3294,7 +3570,7 @@
         <v>106</v>
       </c>
       <c r="K52">
-        <f t="shared" si="0"/>
+        <f>I52/G52</f>
         <v>0.16235427921524026</v>
       </c>
       <c r="M52">
@@ -3330,7 +3606,7 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="K53">
-        <f t="shared" si="0"/>
+        <f>I53/G53</f>
         <v>0.14320154291224688</v>
       </c>
       <c r="M53">
@@ -3366,7 +3642,7 @@
         <v>0.33400000000000002</v>
       </c>
       <c r="K54">
-        <f t="shared" si="0"/>
+        <f>I54/G54</f>
         <v>0.13813068651778329</v>
       </c>
       <c r="M54">
@@ -3402,7 +3678,7 @@
         <v>0.112</v>
       </c>
       <c r="K55">
-        <f t="shared" si="0"/>
+        <f>I55/G55</f>
         <v>0.1761006289308176</v>
       </c>
       <c r="M55">
@@ -3438,7 +3714,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="K56">
-        <f t="shared" si="0"/>
+        <f>I56/G56</f>
         <v>0.29273285568065505</v>
       </c>
       <c r="M56">
@@ -3474,7 +3750,7 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="K57">
-        <f t="shared" si="0"/>
+        <f>I57/G57</f>
         <v>0.1603960396039604</v>
       </c>
       <c r="M57">
@@ -3510,7 +3786,7 @@
         <v>0.127</v>
       </c>
       <c r="K58">
-        <f t="shared" si="0"/>
+        <f>I58/G58</f>
         <v>0.15855181023720349</v>
       </c>
       <c r="L58" t="s">
@@ -3549,7 +3825,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K59">
-        <f t="shared" si="0"/>
+        <f>I59/G59</f>
         <v>0.15204678362573099</v>
       </c>
       <c r="M59">
@@ -3585,7 +3861,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="K60">
-        <f t="shared" si="0"/>
+        <f>I60/G60</f>
         <v>0.14537444933920704</v>
       </c>
       <c r="M60">
@@ -3621,7 +3897,7 @@
         <v>0.08</v>
       </c>
       <c r="K61">
-        <f t="shared" si="0"/>
+        <f>I61/G61</f>
         <v>0.14234875444839856</v>
       </c>
       <c r="M61">
@@ -3657,7 +3933,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="K62">
-        <f t="shared" si="0"/>
+        <f>I62/G62</f>
         <v>0.13892709766162312</v>
       </c>
       <c r="M62">
@@ -3693,7 +3969,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="K63">
-        <f t="shared" si="0"/>
+        <f>I63/G63</f>
         <v>0.1966292134831461</v>
       </c>
       <c r="M63">
@@ -3729,7 +4005,7 @@
         <v>0.499</v>
       </c>
       <c r="K64">
-        <f t="shared" si="0"/>
+        <f>I64/G64</f>
         <v>0.13652530779753763</v>
       </c>
       <c r="M64">
@@ -3765,7 +4041,7 @@
         <v>0.33500000000000002</v>
       </c>
       <c r="K65">
-        <f t="shared" si="0"/>
+        <f>I65/G65</f>
         <v>0.14093395035759362</v>
       </c>
       <c r="M65">
@@ -3801,7 +4077,7 @@
         <v>0.85799999999999998</v>
       </c>
       <c r="K66">
-        <f t="shared" si="0"/>
+        <f>I66/G66</f>
         <v>0.14415322580645162</v>
       </c>
       <c r="M66">
@@ -3837,7 +4113,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K130" si="1">I67/G67</f>
+        <f>I67/G67</f>
         <v>0.11951364175563466</v>
       </c>
       <c r="M67">
@@ -3873,7 +4149,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K68">
-        <f t="shared" si="1"/>
+        <f>I68/G68</f>
         <v>0.18384615384615383</v>
       </c>
       <c r="M68">
@@ -3909,7 +4185,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="K69">
-        <f t="shared" si="1"/>
+        <f>I69/G69</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="M69">
@@ -3945,7 +4221,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="K70">
-        <f t="shared" si="1"/>
+        <f>I70/G70</f>
         <v>0.12992125984251968</v>
       </c>
       <c r="M70">
@@ -3981,7 +4257,7 @@
         <v>0.307</v>
       </c>
       <c r="K71">
-        <f t="shared" si="1"/>
+        <f>I71/G71</f>
         <v>0.15258449304174951</v>
       </c>
       <c r="M71">
@@ -4017,7 +4293,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="K72">
-        <f t="shared" si="1"/>
+        <f>I72/G72</f>
         <v>0.15264797507788161</v>
       </c>
       <c r="M72">
@@ -4053,7 +4329,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="K73">
-        <f t="shared" si="1"/>
+        <f>I73/G73</f>
         <v>0.16569200779727097</v>
       </c>
       <c r="M73">
@@ -4089,7 +4365,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="K74">
-        <f t="shared" si="1"/>
+        <f>I74/G74</f>
         <v>0.26865671641791039</v>
       </c>
       <c r="M74">
@@ -4125,7 +4401,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="K75">
-        <f t="shared" si="1"/>
+        <f>I75/G75</f>
         <v>0.27363184079601988</v>
       </c>
       <c r="M75">
@@ -4161,7 +4437,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="K76">
-        <f t="shared" si="1"/>
+        <f>I76/G76</f>
         <v>0.32926829268292679</v>
       </c>
       <c r="M76">
@@ -4197,7 +4473,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="K77">
-        <f t="shared" si="1"/>
+        <f>I77/G77</f>
         <v>0.17596566523605148</v>
       </c>
       <c r="M77">
@@ -4233,7 +4509,7 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="K78">
-        <f t="shared" si="1"/>
+        <f>I78/G78</f>
         <v>0.17747252747252748</v>
       </c>
       <c r="M78">
@@ -4269,7 +4545,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="K79">
-        <f t="shared" si="1"/>
+        <f>I79/G79</f>
         <v>0.15175995383727639</v>
       </c>
       <c r="M79">
@@ -4305,7 +4581,7 @@
         <v>0.112</v>
       </c>
       <c r="K80">
-        <f t="shared" si="1"/>
+        <f>I80/G80</f>
         <v>0.25168539325842698</v>
       </c>
       <c r="M80">
@@ -4341,7 +4617,7 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="K81">
-        <f t="shared" si="1"/>
+        <f>I81/G81</f>
         <v>0.27878211227402472</v>
       </c>
       <c r="M81">
@@ -4377,7 +4653,7 @@
         <v>0.08</v>
       </c>
       <c r="K82">
-        <f t="shared" si="1"/>
+        <f>I82/G82</f>
         <v>0.31746031746031744</v>
       </c>
       <c r="M82">
@@ -4413,7 +4689,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="K83">
-        <f t="shared" si="1"/>
+        <f>I83/G83</f>
         <v>0.21669106881405562</v>
       </c>
       <c r="M83">
@@ -4449,7 +4725,7 @@
         <v>0.623</v>
       </c>
       <c r="K84">
-        <f t="shared" si="1"/>
+        <f>I84/G84</f>
         <v>0.16653301256348568</v>
       </c>
       <c r="M84">
@@ -4485,7 +4761,7 @@
         <v>0.54800000000000004</v>
       </c>
       <c r="K85">
-        <f t="shared" si="1"/>
+        <f>I85/G85</f>
         <v>0.1928898275255192</v>
       </c>
       <c r="M85">
@@ -4521,7 +4797,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="K86">
-        <f t="shared" si="1"/>
+        <f>I86/G86</f>
         <v>0.16371268656716417</v>
       </c>
       <c r="M86">
@@ -4557,7 +4833,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="K87">
-        <f t="shared" si="1"/>
+        <f>I87/G87</f>
         <v>0.2241813602015113</v>
       </c>
       <c r="M87">
@@ -4593,7 +4869,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="K88">
-        <f t="shared" si="1"/>
+        <f>I88/G88</f>
         <v>0.20634920634920634</v>
       </c>
       <c r="M88">
@@ -4629,7 +4905,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="K89">
-        <f t="shared" si="1"/>
+        <f>I89/G89</f>
         <v>0.21495327102803738</v>
       </c>
       <c r="M89">
@@ -4662,7 +4938,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="K90">
-        <f t="shared" si="1"/>
+        <f>I90/G90</f>
         <v>0.44</v>
       </c>
       <c r="L90" t="s">
@@ -4701,7 +4977,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="K91">
-        <f t="shared" si="1"/>
+        <f>I91/G91</f>
         <v>0.3612903225806452</v>
       </c>
       <c r="M91">
@@ -4737,7 +5013,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K92">
-        <f t="shared" si="1"/>
+        <f>I92/G92</f>
         <v>0.25531914893617019</v>
       </c>
       <c r="M92">
@@ -4773,7 +5049,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K93">
-        <f t="shared" si="1"/>
+        <f>I93/G93</f>
         <v>0.2356020942408377</v>
       </c>
       <c r="M93">
@@ -4809,7 +5085,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="K94">
-        <f t="shared" si="1"/>
+        <f>I94/G94</f>
         <v>0.27066115702479343</v>
       </c>
       <c r="M94">
@@ -4845,7 +5121,7 @@
         <v>0.151</v>
       </c>
       <c r="K95">
-        <f t="shared" si="1"/>
+        <f>I95/G95</f>
         <v>0.24512987012987011</v>
       </c>
       <c r="M95">
@@ -4881,7 +5157,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K96">
-        <f t="shared" si="1"/>
+        <f>I96/G96</f>
         <v>0.273394495412844</v>
       </c>
       <c r="M96">
@@ -4917,7 +5193,7 @@
         <v>0.16</v>
       </c>
       <c r="K97">
-        <f t="shared" si="1"/>
+        <f>I97/G97</f>
         <v>0.31872509960159362</v>
       </c>
       <c r="M97">
@@ -4953,7 +5229,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="K98">
-        <f t="shared" si="1"/>
+        <f>I98/G98</f>
         <v>0.23744292237442921</v>
       </c>
       <c r="M98">
@@ -4989,7 +5265,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="K99">
-        <f t="shared" si="1"/>
+        <f>I99/G99</f>
         <v>0.31720430107526876</v>
       </c>
       <c r="M99">
@@ -5025,7 +5301,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K100">
-        <f t="shared" si="1"/>
+        <f>I100/G100</f>
         <v>0.24792013311148087</v>
       </c>
       <c r="M100">
@@ -5061,7 +5337,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="K101">
-        <f t="shared" si="1"/>
+        <f>I101/G101</f>
         <v>0.13229571984435798</v>
       </c>
       <c r="M101">
@@ -5097,7 +5373,7 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="K102">
-        <f t="shared" si="1"/>
+        <f>I102/G102</f>
         <v>0.21663019693654267</v>
       </c>
       <c r="M102">
@@ -5136,7 +5412,7 @@
         <v>181</v>
       </c>
       <c r="K103">
-        <f t="shared" si="1"/>
+        <f>I103/G103</f>
         <v>0.21598977563192273</v>
       </c>
       <c r="M103">
@@ -5175,7 +5451,7 @@
         <v>183</v>
       </c>
       <c r="K104">
-        <f t="shared" si="1"/>
+        <f>I104/G104</f>
         <v>0.23219597550306212</v>
       </c>
       <c r="M104">
@@ -5211,7 +5487,7 @@
         <v>0.156</v>
       </c>
       <c r="K105">
-        <f t="shared" si="1"/>
+        <f>I105/G105</f>
         <v>0.10303830911492734</v>
       </c>
       <c r="M105">
@@ -5247,7 +5523,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="K106">
-        <f t="shared" si="1"/>
+        <f>I106/G106</f>
         <v>9.7142857142857128E-2</v>
       </c>
       <c r="M106">
@@ -5283,7 +5559,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="K107">
-        <f t="shared" si="1"/>
+        <f>I107/G107</f>
         <v>0.35483870967741932</v>
       </c>
       <c r="M107">
@@ -5319,7 +5595,7 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="K108">
-        <f t="shared" si="1"/>
+        <f>I108/G108</f>
         <v>0.16381418092909539</v>
       </c>
       <c r="M108">
@@ -5355,7 +5631,7 @@
         <v>0.188</v>
       </c>
       <c r="K109">
-        <f t="shared" si="1"/>
+        <f>I109/G109</f>
         <v>0.1407185628742515</v>
       </c>
       <c r="M109">
@@ -5391,7 +5667,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="K110">
-        <f t="shared" si="1"/>
+        <f>I110/G110</f>
         <v>0.25</v>
       </c>
       <c r="M110">
@@ -5427,7 +5703,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="K111">
-        <f t="shared" si="1"/>
+        <f>I111/G111</f>
         <v>0.23008849557522121</v>
       </c>
       <c r="M111">
@@ -5463,7 +5739,7 @@
         <v>0.111</v>
       </c>
       <c r="K112">
-        <f t="shared" si="1"/>
+        <f>I112/G112</f>
         <v>0.22560975609756098</v>
       </c>
       <c r="M112">
@@ -5499,7 +5775,7 @@
         <v>0.35499999999999998</v>
       </c>
       <c r="K113">
-        <f t="shared" si="1"/>
+        <f>I113/G113</f>
         <v>0.13878029710711492</v>
       </c>
       <c r="M113">
@@ -5535,7 +5811,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K114">
-        <f t="shared" si="1"/>
+        <f>I114/G114</f>
         <v>0.14216084484159219</v>
       </c>
       <c r="M114">
@@ -5571,7 +5847,7 @@
         <v>0.248</v>
       </c>
       <c r="K115">
-        <f t="shared" si="1"/>
+        <f>I115/G115</f>
         <v>0.15432482887367766</v>
       </c>
       <c r="M115">
@@ -5607,7 +5883,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="K116">
-        <f t="shared" si="1"/>
+        <f>I116/G116</f>
         <v>0.10258302583025831</v>
       </c>
       <c r="M116">
@@ -5643,7 +5919,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="K117">
-        <f t="shared" si="1"/>
+        <f>I117/G117</f>
         <v>8.6854460093896718E-2</v>
       </c>
       <c r="M117">
@@ -5679,7 +5955,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K118">
-        <f t="shared" si="1"/>
+        <f>I118/G118</f>
         <v>8.3597883597883602E-2</v>
       </c>
       <c r="M118">
@@ -5718,7 +5994,7 @@
         <v>201</v>
       </c>
       <c r="K119">
-        <f t="shared" si="1"/>
+        <f>I119/G119</f>
         <v>0.19229638341664218</v>
       </c>
       <c r="M119">
@@ -5754,7 +6030,7 @@
         <v>0.155</v>
       </c>
       <c r="K120">
-        <f t="shared" si="1"/>
+        <f>I120/G120</f>
         <v>0.16028955532574973</v>
       </c>
       <c r="M120">
@@ -5790,7 +6066,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="K121">
-        <f t="shared" si="1"/>
+        <f>I121/G121</f>
         <v>0.15618521078092606</v>
       </c>
       <c r="M121">
@@ -5826,7 +6102,7 @@
         <v>0.89800000000000002</v>
       </c>
       <c r="K122">
-        <f t="shared" si="1"/>
+        <f>I122/G122</f>
         <v>0.20293785310734463</v>
       </c>
       <c r="M122">
@@ -5862,7 +6138,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="K123">
-        <f t="shared" si="1"/>
+        <f>I123/G123</f>
         <v>0.36999999999999994</v>
       </c>
       <c r="M123">
@@ -5901,7 +6177,7 @@
         <v>207</v>
       </c>
       <c r="K124">
-        <f t="shared" si="1"/>
+        <f>I124/G124</f>
         <v>0.24628635626014234</v>
       </c>
       <c r="M124">
@@ -5937,7 +6213,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K125">
-        <f t="shared" si="1"/>
+        <f>I125/G125</f>
         <v>0.3428571428571428</v>
       </c>
       <c r="M125">
@@ -5973,7 +6249,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="K126">
-        <f t="shared" si="1"/>
+        <f>I126/G126</f>
         <v>0.3146067415730337</v>
       </c>
       <c r="M126">
@@ -6009,7 +6285,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K127">
-        <f t="shared" si="1"/>
+        <f>I127/G127</f>
         <v>0.32500000000000001</v>
       </c>
       <c r="M127">
@@ -6045,7 +6321,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K128">
-        <f t="shared" si="1"/>
+        <f>I128/G128</f>
         <v>0.27916666666666667</v>
       </c>
       <c r="M128">
@@ -6081,7 +6357,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="K129">
-        <f t="shared" si="1"/>
+        <f>I129/G129</f>
         <v>0.25405405405405407</v>
       </c>
       <c r="M129">
@@ -6117,7 +6393,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K130">
-        <f t="shared" si="1"/>
+        <f>I130/G130</f>
         <v>0.29545454545454541</v>
       </c>
       <c r="M130">
@@ -6153,7 +6429,7 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="K131">
-        <f t="shared" ref="K131:K217" si="2">I131/G131</f>
+        <f>I131/G131</f>
         <v>0.20935861234368697</v>
       </c>
       <c r="M131">
@@ -6189,7 +6465,7 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="K132">
-        <f t="shared" si="2"/>
+        <f>I132/G132</f>
         <v>0.2050805452292441</v>
       </c>
       <c r="M132">
@@ -6225,7 +6501,7 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="K133">
-        <f t="shared" si="2"/>
+        <f>I133/G133</f>
         <v>0.16473551637279596</v>
       </c>
       <c r="M133">
@@ -6261,7 +6537,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="K134">
-        <f t="shared" si="2"/>
+        <f>I134/G134</f>
         <v>0.32</v>
       </c>
       <c r="M134">
@@ -6297,7 +6573,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="K135">
-        <f t="shared" si="2"/>
+        <f>I135/G135</f>
         <v>0.29870129870129869</v>
       </c>
       <c r="M135">
@@ -6333,7 +6609,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="K136">
-        <f t="shared" si="2"/>
+        <f>I136/G136</f>
         <v>0.28629032258064513</v>
       </c>
       <c r="M136">
@@ -6369,7 +6645,7 @@
         <v>0.39300000000000002</v>
       </c>
       <c r="K137">
-        <f t="shared" si="2"/>
+        <f>I137/G137</f>
         <v>0.4145569620253165</v>
       </c>
       <c r="M137">
@@ -6405,7 +6681,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="K138">
-        <f t="shared" si="2"/>
+        <f>I138/G138</f>
         <v>0.1956368754398311</v>
       </c>
       <c r="M138">
@@ -6441,7 +6717,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K139">
-        <f t="shared" si="2"/>
+        <f>I139/G139</f>
         <v>0.18233082706766918</v>
       </c>
       <c r="M139">
@@ -6477,7 +6753,7 @@
         <v>0.15</v>
       </c>
       <c r="K140">
-        <f t="shared" si="2"/>
+        <f>I140/G140</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="M140">
@@ -6513,7 +6789,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="K141">
-        <f t="shared" si="2"/>
+        <f>I141/G141</f>
         <v>0.20417633410672853</v>
       </c>
       <c r="M141">
@@ -6549,7 +6825,7 @@
         <v>0.108</v>
       </c>
       <c r="K142">
-        <f t="shared" si="2"/>
+        <f>I142/G142</f>
         <v>0.20650095602294455</v>
       </c>
       <c r="M142">
@@ -6585,7 +6861,7 @@
         <v>0.314</v>
       </c>
       <c r="K143">
-        <f t="shared" si="2"/>
+        <f>I143/G143</f>
         <v>0.21820708825573315</v>
       </c>
       <c r="M143">
@@ -6621,7 +6897,7 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="K144">
-        <f t="shared" si="2"/>
+        <f>I144/G144</f>
         <v>0.20233463035019453</v>
       </c>
       <c r="M144">
@@ -6657,7 +6933,7 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="K145">
-        <f t="shared" si="2"/>
+        <f>I145/G145</f>
         <v>0.21382488479262673</v>
       </c>
       <c r="M145">
@@ -6693,7 +6969,7 @@
         <v>0.35899999999999999</v>
       </c>
       <c r="K146">
-        <f t="shared" si="2"/>
+        <f>I146/G146</f>
         <v>0.19638949671772427</v>
       </c>
       <c r="M146">
@@ -6729,7 +7005,7 @@
         <v>0.54</v>
       </c>
       <c r="K147">
-        <f t="shared" si="2"/>
+        <f>I147/G147</f>
         <v>0.21827000808407437</v>
       </c>
       <c r="M147">
@@ -6765,7 +7041,7 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="K148">
-        <f t="shared" si="2"/>
+        <f>I148/G148</f>
         <v>0.19671132764920829</v>
       </c>
       <c r="M148">
@@ -6801,7 +7077,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="K149">
-        <f t="shared" si="2"/>
+        <f>I149/G149</f>
         <v>0.17678868552412647</v>
       </c>
       <c r="M149">
@@ -6837,7 +7113,7 @@
         <v>0.49399999999999999</v>
       </c>
       <c r="K150">
-        <f t="shared" si="2"/>
+        <f>I150/G150</f>
         <v>0.17333333333333334</v>
       </c>
       <c r="M150">
@@ -6873,7 +7149,7 @@
         <v>0.188</v>
       </c>
       <c r="K151">
-        <f t="shared" si="2"/>
+        <f>I151/G151</f>
         <v>0.19282051282051282</v>
       </c>
       <c r="M151">
@@ -6909,7 +7185,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K152">
-        <f t="shared" si="2"/>
+        <f>I152/G152</f>
         <v>0.18210459987397604</v>
       </c>
       <c r="M152">
@@ -6945,7 +7221,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="K153">
-        <f t="shared" si="2"/>
+        <f>I153/G153</f>
         <v>0.18114406779661019</v>
       </c>
       <c r="M153">
@@ -6981,7 +7257,7 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="K154">
-        <f t="shared" si="2"/>
+        <f>I154/G154</f>
         <v>9.9956350938454827E-2</v>
       </c>
       <c r="M154">
@@ -7020,7 +7296,7 @@
         <v>257</v>
       </c>
       <c r="K155">
-        <f t="shared" si="2"/>
+        <f>I155/G155</f>
         <v>0.10982286634460547</v>
       </c>
       <c r="M155">
@@ -7059,7 +7335,7 @@
         <v>259</v>
       </c>
       <c r="K156">
-        <f t="shared" si="2"/>
+        <f>I156/G156</f>
         <v>0.10955686065136146</v>
       </c>
       <c r="M156">
@@ -7095,7 +7371,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="K157">
-        <f t="shared" si="2"/>
+        <f>I157/G157</f>
         <v>0.10804911323328786</v>
       </c>
       <c r="M157">
@@ -7134,7 +7410,7 @@
         <v>262</v>
       </c>
       <c r="K158">
-        <f t="shared" si="2"/>
+        <f>I158/G158</f>
         <v>0.10712166172106824</v>
       </c>
       <c r="M158">
@@ -7170,7 +7446,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="K159">
-        <f t="shared" si="2"/>
+        <f>I159/G159</f>
         <v>0.15313653136531366</v>
       </c>
       <c r="M159">
@@ -7206,7 +7482,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K160">
-        <f t="shared" si="2"/>
+        <f>I160/G160</f>
         <v>0.16421052631578947</v>
       </c>
       <c r="M160">
@@ -7242,7 +7518,7 @@
         <v>0.05</v>
       </c>
       <c r="K161">
-        <f t="shared" si="2"/>
+        <f>I161/G161</f>
         <v>0.15060240963855423</v>
       </c>
       <c r="M161">
@@ -7278,7 +7554,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="K162">
-        <f t="shared" si="2"/>
+        <f>I162/G162</f>
         <v>0.13989637305699482</v>
       </c>
       <c r="M162">
@@ -7314,7 +7590,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K163">
-        <f t="shared" si="2"/>
+        <f>I163/G163</f>
         <v>0.13483146067415727</v>
       </c>
       <c r="M163">
@@ -7350,7 +7626,7 @@
         <v>0.36399999999999999</v>
       </c>
       <c r="K164">
-        <f t="shared" si="2"/>
+        <f>I164/G164</f>
         <v>0.20289855072463767</v>
       </c>
       <c r="M164">
@@ -7386,7 +7662,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="K165">
-        <f t="shared" si="2"/>
+        <f>I165/G165</f>
         <v>0.14890282131661442</v>
       </c>
       <c r="M165">
@@ -7422,7 +7698,7 @@
         <v>0.11</v>
       </c>
       <c r="K166">
-        <f t="shared" si="2"/>
+        <f>I166/G166</f>
         <v>0.13253012048192772</v>
       </c>
       <c r="M166">
@@ -7458,7 +7734,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K167">
-        <f t="shared" si="2"/>
+        <f>I167/G167</f>
         <v>0.1296625222024867</v>
       </c>
       <c r="M167">
@@ -7494,7 +7770,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="K168">
-        <f t="shared" si="2"/>
+        <f>I168/G168</f>
         <v>0.18580645161290321</v>
       </c>
       <c r="M168">
@@ -7530,7 +7806,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K169">
-        <f t="shared" si="2"/>
+        <f>I169/G169</f>
         <v>0.19367909238249595</v>
       </c>
       <c r="M169">
@@ -7566,7 +7842,7 @@
         <v>0.153</v>
       </c>
       <c r="K170">
-        <f t="shared" si="2"/>
+        <f>I170/G170</f>
         <v>0.18635809987819732</v>
       </c>
       <c r="M170">
@@ -7602,7 +7878,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="K171">
-        <f t="shared" si="2"/>
+        <f>I171/G171</f>
         <v>0.18611987381703471</v>
       </c>
       <c r="M171">
@@ -7638,7 +7914,7 @@
         <v>0.25</v>
       </c>
       <c r="K172">
-        <f t="shared" si="2"/>
+        <f>I172/G172</f>
         <v>0.19762845849802374</v>
       </c>
       <c r="M172">
@@ -7674,7 +7950,7 @@
         <v>0.84799999999999998</v>
       </c>
       <c r="K173">
-        <f t="shared" si="2"/>
+        <f>I173/G173</f>
         <v>6.8260484585043871E-2</v>
       </c>
       <c r="M173">
@@ -7710,7 +7986,7 @@
         <v>1.036</v>
       </c>
       <c r="K174">
-        <f t="shared" si="2"/>
+        <f>I174/G174</f>
         <v>7.7353841559023376E-2</v>
       </c>
       <c r="M174">
@@ -7746,7 +8022,7 @@
         <v>0.42599999999999999</v>
       </c>
       <c r="K175">
-        <f t="shared" si="2"/>
+        <f>I175/G175</f>
         <v>9.1731266149870802E-2</v>
       </c>
       <c r="M175">
@@ -7782,7 +8058,7 @@
         <v>0.60499999999999998</v>
       </c>
       <c r="K176">
-        <f t="shared" si="2"/>
+        <f>I176/G176</f>
         <v>8.5355530474040625E-2</v>
       </c>
       <c r="M176">
@@ -7818,7 +8094,7 @@
         <v>0.63</v>
       </c>
       <c r="K177">
-        <f t="shared" si="2"/>
+        <f>I177/G177</f>
         <v>7.6754385964912283E-2</v>
       </c>
       <c r="M177">
@@ -7854,7 +8130,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="K178">
-        <f t="shared" si="2"/>
+        <f>I178/G178</f>
         <v>0.24358974358974358</v>
       </c>
       <c r="M178">
@@ -7890,7 +8166,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K179">
-        <f t="shared" si="2"/>
+        <f>I179/G179</f>
         <v>0.23076923076923075</v>
       </c>
       <c r="M179">
@@ -7926,7 +8202,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K180">
-        <f t="shared" si="2"/>
+        <f>I180/G180</f>
         <v>0.210412147505423</v>
       </c>
       <c r="M180">
@@ -7962,7 +8238,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K181">
-        <f t="shared" si="2"/>
+        <f>I181/G181</f>
         <v>0.25</v>
       </c>
       <c r="M181">
@@ -7998,7 +8274,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="K182">
-        <f t="shared" si="2"/>
+        <f>I182/G182</f>
         <v>0.19375000000000001</v>
       </c>
       <c r="M182">
@@ -8034,7 +8310,7 @@
         <v>0.127</v>
       </c>
       <c r="K183">
-        <f t="shared" si="2"/>
+        <f>I183/G183</f>
         <v>0.22678571428571426</v>
       </c>
       <c r="M183">
@@ -8070,7 +8346,7 @@
         <v>0.158</v>
       </c>
       <c r="K184">
-        <f t="shared" si="2"/>
+        <f>I184/G184</f>
         <v>0.22067039106145253</v>
       </c>
       <c r="M184">
@@ -8106,7 +8382,7 @@
         <v>0.159</v>
       </c>
       <c r="K185">
-        <f t="shared" si="2"/>
+        <f>I185/G185</f>
         <v>0.24164133738601823</v>
       </c>
       <c r="M185">
@@ -8142,7 +8418,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="K186">
-        <f t="shared" si="2"/>
+        <f>I186/G186</f>
         <v>0.21549421193232413</v>
       </c>
       <c r="M186">
@@ -8178,7 +8454,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="K187">
-        <f t="shared" si="2"/>
+        <f>I187/G187</f>
         <v>0.15271493212669685</v>
       </c>
       <c r="M187">
@@ -8214,7 +8490,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="K188">
-        <f t="shared" si="2"/>
+        <f>I188/G188</f>
         <v>0.15111111111111111</v>
       </c>
       <c r="M188">
@@ -8250,7 +8526,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K189">
-        <f t="shared" si="2"/>
+        <f>I189/G189</f>
         <v>0.13688212927756652</v>
       </c>
       <c r="M189">
@@ -8286,7 +8562,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K190">
-        <f t="shared" si="2"/>
+        <f>I190/G190</f>
         <v>0.15837104072398189</v>
       </c>
       <c r="M190">
@@ -8322,7 +8598,7 @@
         <v>0.112</v>
       </c>
       <c r="K191">
-        <f t="shared" si="2"/>
+        <f>I191/G191</f>
         <v>0.13559322033898305</v>
       </c>
       <c r="M191">
@@ -8358,7 +8634,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K192">
-        <f t="shared" si="2"/>
+        <f>I192/G192</f>
         <v>0.12324492979719189</v>
       </c>
       <c r="M192">
@@ -8394,7 +8670,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="K193">
-        <f t="shared" si="2"/>
+        <f>I193/G193</f>
         <v>0.16300940438871472</v>
       </c>
       <c r="M193">
@@ -8430,7 +8706,7 @@
         <v>0.124</v>
       </c>
       <c r="K194">
-        <f t="shared" si="2"/>
+        <f>I194/G194</f>
         <v>0.15066828675577157</v>
       </c>
       <c r="M194">
@@ -8466,7 +8742,7 @@
         <v>0.113</v>
       </c>
       <c r="K195">
-        <f t="shared" si="2"/>
+        <f>I195/G195</f>
         <v>0.13647342995169084</v>
       </c>
       <c r="M195">
@@ -8502,7 +8778,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="K196">
-        <f t="shared" si="2"/>
+        <f>I196/G196</f>
         <v>0.17346938775510204</v>
       </c>
       <c r="M196">
@@ -8538,7 +8814,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="K197">
-        <f t="shared" si="2"/>
+        <f>I197/G197</f>
         <v>0.17375886524822695</v>
       </c>
       <c r="M197">
@@ -8574,7 +8850,7 @@
         <v>0.03</v>
       </c>
       <c r="K198">
-        <f t="shared" si="2"/>
+        <f>I198/G198</f>
         <v>0.19480519480519479</v>
       </c>
       <c r="M198">
@@ -8610,7 +8886,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="K199">
-        <f t="shared" si="2"/>
+        <f>I199/G199</f>
         <v>0.178343949044586</v>
       </c>
       <c r="M199">
@@ -8646,7 +8922,7 @@
         <v>0.217</v>
       </c>
       <c r="K200">
-        <f t="shared" si="2"/>
+        <f>I200/G200</f>
         <v>0.16476841305998483</v>
       </c>
       <c r="M200">
@@ -8682,7 +8958,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K201">
-        <f t="shared" si="2"/>
+        <f>I201/G201</f>
         <v>0.14272030651340994</v>
       </c>
       <c r="M201">
@@ -8718,7 +8994,7 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="K202">
-        <f t="shared" si="2"/>
+        <f>I202/G202</f>
         <v>0.15776699029126215</v>
       </c>
       <c r="M202">
@@ -8754,7 +9030,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="K203">
-        <f t="shared" si="2"/>
+        <f>I203/G203</f>
         <v>0.12428842504743833</v>
       </c>
       <c r="M203">
@@ -8790,7 +9066,7 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="K204">
-        <f t="shared" si="2"/>
+        <f>I204/G204</f>
         <v>0.13804971319311662</v>
       </c>
       <c r="M204">
@@ -8826,7 +9102,7 @@
         <v>0.189</v>
       </c>
       <c r="K205">
-        <f t="shared" si="2"/>
+        <f>I205/G205</f>
         <v>0.13815789473684209</v>
       </c>
       <c r="M205">
@@ -8862,7 +9138,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K206">
-        <f t="shared" si="2"/>
+        <f>I206/G206</f>
         <v>0.1411822178798241</v>
       </c>
       <c r="M206">
@@ -8898,7 +9174,7 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="K207">
-        <f t="shared" si="2"/>
+        <f>I207/G207</f>
         <v>0.12414042707202318</v>
       </c>
       <c r="M207">
@@ -8934,7 +9210,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="K208">
-        <f t="shared" si="2"/>
+        <f>I208/G208</f>
         <v>0.13170272812793982</v>
       </c>
       <c r="M208">
@@ -8970,7 +9246,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="K209">
-        <f t="shared" si="2"/>
+        <f>I209/G209</f>
         <v>0.12742812742812745</v>
       </c>
       <c r="M209">
@@ -9006,7 +9282,7 @@
         <v>0.12</v>
       </c>
       <c r="K210">
-        <f t="shared" si="2"/>
+        <f>I210/G210</f>
         <v>0.19108280254777069</v>
       </c>
       <c r="M210">
@@ -9042,7 +9318,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="K211">
-        <f t="shared" si="2"/>
+        <f>I211/G211</f>
         <v>0.20435967302452315</v>
       </c>
       <c r="M211">
@@ -9078,7 +9354,7 @@
         <v>0.05</v>
       </c>
       <c r="K212">
-        <f t="shared" si="2"/>
+        <f>I212/G212</f>
         <v>0.2183406113537118</v>
       </c>
       <c r="M212">
@@ -9117,7 +9393,7 @@
         <v>329</v>
       </c>
       <c r="K213">
-        <f t="shared" si="2"/>
+        <f>I213/G213</f>
         <v>0.12863436123348018</v>
       </c>
       <c r="M213">
@@ -9153,7 +9429,7 @@
         <v>0.69499999999999995</v>
       </c>
       <c r="K214">
-        <f t="shared" si="2"/>
+        <f>I214/G214</f>
         <v>0.11831801157643854</v>
       </c>
       <c r="M214">
@@ -9192,7 +9468,7 @@
         <v>332</v>
       </c>
       <c r="K215">
-        <f t="shared" si="2"/>
+        <f>I215/G215</f>
         <v>0.12973508294132211</v>
       </c>
       <c r="M215">
@@ -9228,7 +9504,7 @@
         <v>0.53300000000000003</v>
       </c>
       <c r="K216">
-        <f t="shared" si="2"/>
+        <f>I216/G216</f>
         <v>0.11162303664921466</v>
       </c>
       <c r="M216">
@@ -9264,11 +9540,2681 @@
         <v>0.66900000000000004</v>
       </c>
       <c r="K217">
-        <f t="shared" si="2"/>
+        <f>I217/G217</f>
         <v>7.5253093363329582E-2</v>
       </c>
       <c r="M217">
         <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>50</v>
+      </c>
+      <c r="B218" t="s">
+        <v>335</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D218" t="s">
+        <v>337</v>
+      </c>
+      <c r="E218">
+        <v>10</v>
+      </c>
+      <c r="F218">
+        <v>3</v>
+      </c>
+      <c r="G218">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H218" t="s">
+        <v>338</v>
+      </c>
+      <c r="I218">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K218">
+        <f>I218/G218</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="M218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>50</v>
+      </c>
+      <c r="B219" t="s">
+        <v>335</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D219" t="s">
+        <v>337</v>
+      </c>
+      <c r="E219">
+        <v>9</v>
+      </c>
+      <c r="F219">
+        <v>5</v>
+      </c>
+      <c r="G219">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="H219" t="s">
+        <v>339</v>
+      </c>
+      <c r="I219">
+        <v>0.128</v>
+      </c>
+      <c r="K219">
+        <f>I219/G219</f>
+        <v>0.24854368932038834</v>
+      </c>
+      <c r="M219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>50</v>
+      </c>
+      <c r="B220" t="s">
+        <v>335</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D220" t="s">
+        <v>337</v>
+      </c>
+      <c r="E220">
+        <v>8</v>
+      </c>
+      <c r="F220">
+        <v>3</v>
+      </c>
+      <c r="G220">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="H220" t="s">
+        <v>340</v>
+      </c>
+      <c r="I220">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K220">
+        <f>I220/G220</f>
+        <v>0.24781341107871721</v>
+      </c>
+      <c r="M220">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>50</v>
+      </c>
+      <c r="B221" t="s">
+        <v>335</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D221" t="s">
+        <v>337</v>
+      </c>
+      <c r="E221">
+        <v>7</v>
+      </c>
+      <c r="F221">
+        <v>4</v>
+      </c>
+      <c r="G221">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="H221" t="s">
+        <v>341</v>
+      </c>
+      <c r="I221">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="K221">
+        <f>I221/G221</f>
+        <v>0.23268698060941831</v>
+      </c>
+      <c r="M221">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>50</v>
+      </c>
+      <c r="B222" t="s">
+        <v>335</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D222" t="s">
+        <v>337</v>
+      </c>
+      <c r="E222">
+        <v>6</v>
+      </c>
+      <c r="F222">
+        <v>2</v>
+      </c>
+      <c r="G222">
+        <v>0.371</v>
+      </c>
+      <c r="H222" t="s">
+        <v>342</v>
+      </c>
+      <c r="I222">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="K222">
+        <f>I222/G222</f>
+        <v>0.23719676549865229</v>
+      </c>
+      <c r="M222">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>50</v>
+      </c>
+      <c r="B223" t="s">
+        <v>335</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D223" t="s">
+        <v>337</v>
+      </c>
+      <c r="E223">
+        <v>5</v>
+      </c>
+      <c r="F223">
+        <v>3</v>
+      </c>
+      <c r="G223">
+        <v>0.77</v>
+      </c>
+      <c r="H223" t="s">
+        <v>343</v>
+      </c>
+      <c r="I223">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="K223">
+        <f>I223/G223</f>
+        <v>0.25454545454545457</v>
+      </c>
+      <c r="M223">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>50</v>
+      </c>
+      <c r="B224" t="s">
+        <v>335</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D224" t="s">
+        <v>337</v>
+      </c>
+      <c r="E224">
+        <v>4</v>
+      </c>
+      <c r="F224">
+        <v>5</v>
+      </c>
+      <c r="G224">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H224" t="s">
+        <v>344</v>
+      </c>
+      <c r="I224">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K224">
+        <f>I224/G224</f>
+        <v>0.23529411764705885</v>
+      </c>
+      <c r="M224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>50</v>
+      </c>
+      <c r="B225" t="s">
+        <v>335</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D225" t="s">
+        <v>337</v>
+      </c>
+      <c r="E225">
+        <v>3</v>
+      </c>
+      <c r="F225">
+        <v>3</v>
+      </c>
+      <c r="G225">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="H225" t="s">
+        <v>345</v>
+      </c>
+      <c r="I225">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="K225">
+        <f>I225/G225</f>
+        <v>0.24277456647398848</v>
+      </c>
+      <c r="M225">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>50</v>
+      </c>
+      <c r="B226" t="s">
+        <v>335</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D226" t="s">
+        <v>337</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="F226">
+        <v>2</v>
+      </c>
+      <c r="G226">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="H226" t="s">
+        <v>346</v>
+      </c>
+      <c r="I226">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="K226">
+        <f>I226/G226</f>
+        <v>0.27492447129909364</v>
+      </c>
+      <c r="M226">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>50</v>
+      </c>
+      <c r="B227" t="s">
+        <v>335</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D227" t="s">
+        <v>337</v>
+      </c>
+      <c r="E227">
+        <v>1</v>
+      </c>
+      <c r="F227">
+        <v>5</v>
+      </c>
+      <c r="G227">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="H227" t="s">
+        <v>347</v>
+      </c>
+      <c r="I227">
+        <v>0.1</v>
+      </c>
+      <c r="K227">
+        <f>I227/G227</f>
+        <v>0.24330900243309006</v>
+      </c>
+      <c r="M227">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>74</v>
+      </c>
+      <c r="B228" t="s">
+        <v>75</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D228" t="s">
+        <v>349</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+      <c r="F228">
+        <v>4</v>
+      </c>
+      <c r="G228">
+        <v>1.024</v>
+      </c>
+      <c r="H228" t="s">
+        <v>350</v>
+      </c>
+      <c r="I228">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="K228">
+        <f>I228/G228</f>
+        <v>0.1669921875</v>
+      </c>
+      <c r="M228">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>74</v>
+      </c>
+      <c r="B229" t="s">
+        <v>75</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D229" t="s">
+        <v>349</v>
+      </c>
+      <c r="E229">
+        <v>2</v>
+      </c>
+      <c r="F229">
+        <v>5</v>
+      </c>
+      <c r="G229">
+        <v>1.488</v>
+      </c>
+      <c r="H229" t="s">
+        <v>351</v>
+      </c>
+      <c r="I229">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K229">
+        <f>I229/G229</f>
+        <v>0.15793010752688172</v>
+      </c>
+      <c r="M229">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>74</v>
+      </c>
+      <c r="B230" t="s">
+        <v>75</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D230" t="s">
+        <v>349</v>
+      </c>
+      <c r="E230">
+        <v>3</v>
+      </c>
+      <c r="F230">
+        <v>7</v>
+      </c>
+      <c r="G230">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="H230" t="s">
+        <v>352</v>
+      </c>
+      <c r="I230">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="K230">
+        <f>I230/G230</f>
+        <v>0.15300146412884333</v>
+      </c>
+      <c r="M230">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>74</v>
+      </c>
+      <c r="B231" t="s">
+        <v>75</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D231" t="s">
+        <v>349</v>
+      </c>
+      <c r="E231">
+        <v>4</v>
+      </c>
+      <c r="F231">
+        <v>5</v>
+      </c>
+      <c r="G231">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="H231" t="s">
+        <v>353</v>
+      </c>
+      <c r="I231">
+        <v>0.124</v>
+      </c>
+      <c r="K231">
+        <f>I231/G231</f>
+        <v>0.16916780354706684</v>
+      </c>
+      <c r="M231">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>149</v>
+      </c>
+      <c r="B232" t="s">
+        <v>168</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D232" t="s">
+        <v>349</v>
+      </c>
+      <c r="E232">
+        <v>1</v>
+      </c>
+      <c r="F232">
+        <v>7</v>
+      </c>
+      <c r="G232">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="H232" t="s">
+        <v>354</v>
+      </c>
+      <c r="I232">
+        <v>0.121</v>
+      </c>
+      <c r="K232">
+        <f>I232/G232</f>
+        <v>0.19803600654664485</v>
+      </c>
+      <c r="M232">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>149</v>
+      </c>
+      <c r="B233" t="s">
+        <v>168</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D233" t="s">
+        <v>349</v>
+      </c>
+      <c r="E233">
+        <v>2</v>
+      </c>
+      <c r="F233">
+        <v>3</v>
+      </c>
+      <c r="G233">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H233" t="s">
+        <v>355</v>
+      </c>
+      <c r="I233">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K233">
+        <f>I233/G233</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="M233">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>29</v>
+      </c>
+      <c r="B234" t="s">
+        <v>30</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D234" t="s">
+        <v>356</v>
+      </c>
+      <c r="E234">
+        <v>1</v>
+      </c>
+      <c r="F234">
+        <v>5</v>
+      </c>
+      <c r="G234">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H234" t="s">
+        <v>357</v>
+      </c>
+      <c r="I234">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="K234">
+        <f>I234/G234</f>
+        <v>0.26909090909090905</v>
+      </c>
+      <c r="M234">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>29</v>
+      </c>
+      <c r="B235" t="s">
+        <v>30</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D235" t="s">
+        <v>356</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+      <c r="F235">
+        <v>5</v>
+      </c>
+      <c r="G235">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="H235" t="s">
+        <v>358</v>
+      </c>
+      <c r="I235">
+        <v>0.18</v>
+      </c>
+      <c r="K235">
+        <f>I235/G235</f>
+        <v>0.20134228187919462</v>
+      </c>
+      <c r="M235">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>29</v>
+      </c>
+      <c r="B236" t="s">
+        <v>30</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D236" t="s">
+        <v>356</v>
+      </c>
+      <c r="E236">
+        <v>3</v>
+      </c>
+      <c r="F236">
+        <v>4</v>
+      </c>
+      <c r="G236">
+        <v>1.004</v>
+      </c>
+      <c r="H236" t="s">
+        <v>359</v>
+      </c>
+      <c r="I236">
+        <v>0.223</v>
+      </c>
+      <c r="K236">
+        <f>I236/G236</f>
+        <v>0.22211155378486055</v>
+      </c>
+      <c r="M236">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>29</v>
+      </c>
+      <c r="B237" t="s">
+        <v>30</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D237" t="s">
+        <v>356</v>
+      </c>
+      <c r="E237">
+        <v>4</v>
+      </c>
+      <c r="F237">
+        <v>5</v>
+      </c>
+      <c r="G237">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="H237" t="s">
+        <v>360</v>
+      </c>
+      <c r="I237">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="K237">
+        <f>I237/G237</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="M237">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>149</v>
+      </c>
+      <c r="B238" t="s">
+        <v>150</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D238" t="s">
+        <v>356</v>
+      </c>
+      <c r="E238">
+        <v>1</v>
+      </c>
+      <c r="F238">
+        <v>6</v>
+      </c>
+      <c r="G238">
+        <v>1.7609999999999999</v>
+      </c>
+      <c r="H238" t="s">
+        <v>361</v>
+      </c>
+      <c r="I238">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="K238">
+        <f>I238/G238</f>
+        <v>0.18285065303804657</v>
+      </c>
+      <c r="M238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>149</v>
+      </c>
+      <c r="B239" t="s">
+        <v>150</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D239" t="s">
+        <v>356</v>
+      </c>
+      <c r="E239">
+        <v>2</v>
+      </c>
+      <c r="F239">
+        <v>5</v>
+      </c>
+      <c r="G239">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="H239" t="s">
+        <v>362</v>
+      </c>
+      <c r="I239">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="K239">
+        <f>I239/G239</f>
+        <v>0.20364920541494994</v>
+      </c>
+      <c r="M239">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>149</v>
+      </c>
+      <c r="B240" t="s">
+        <v>150</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D240" t="s">
+        <v>356</v>
+      </c>
+      <c r="E240">
+        <v>3</v>
+      </c>
+      <c r="F240">
+        <v>5</v>
+      </c>
+      <c r="G240">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="H240" t="s">
+        <v>363</v>
+      </c>
+      <c r="I240">
+        <v>0.307</v>
+      </c>
+      <c r="K240">
+        <f>I240/G240</f>
+        <v>0.20398671096345516</v>
+      </c>
+      <c r="M240">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>287</v>
+      </c>
+      <c r="B241" t="s">
+        <v>288</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D241" t="s">
+        <v>337</v>
+      </c>
+      <c r="E241">
+        <v>2</v>
+      </c>
+      <c r="F241">
+        <v>3</v>
+      </c>
+      <c r="G241">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="H241" t="s">
+        <v>364</v>
+      </c>
+      <c r="I241">
+        <v>0.253</v>
+      </c>
+      <c r="K241">
+        <f>I241/G241</f>
+        <v>0.20891824938067713</v>
+      </c>
+      <c r="M241">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>287</v>
+      </c>
+      <c r="B242" t="s">
+        <v>288</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D242" t="s">
+        <v>337</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="F242">
+        <v>3</v>
+      </c>
+      <c r="G242">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="H242" t="s">
+        <v>365</v>
+      </c>
+      <c r="I242">
+        <v>0.126</v>
+      </c>
+      <c r="K242">
+        <f>I242/G242</f>
+        <v>0.2475442043222004</v>
+      </c>
+      <c r="M242">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>366</v>
+      </c>
+      <c r="B243" t="s">
+        <v>367</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D243" t="s">
+        <v>368</v>
+      </c>
+      <c r="E243">
+        <v>1</v>
+      </c>
+      <c r="F243">
+        <v>7</v>
+      </c>
+      <c r="G243">
+        <v>0.19</v>
+      </c>
+      <c r="H243" t="s">
+        <v>369</v>
+      </c>
+      <c r="I243">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="K243">
+        <f>I243/G243</f>
+        <v>0.22105263157894739</v>
+      </c>
+      <c r="M243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>366</v>
+      </c>
+      <c r="B244" t="s">
+        <v>367</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D244" t="s">
+        <v>356</v>
+      </c>
+      <c r="E244">
+        <v>2</v>
+      </c>
+      <c r="F244">
+        <v>7</v>
+      </c>
+      <c r="G244">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H244" t="s">
+        <v>370</v>
+      </c>
+      <c r="I244">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="K244">
+        <f>I244/G244</f>
+        <v>0.22564102564102562</v>
+      </c>
+      <c r="M244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>366</v>
+      </c>
+      <c r="B245" t="s">
+        <v>367</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D245" t="s">
+        <v>356</v>
+      </c>
+      <c r="E245">
+        <v>3</v>
+      </c>
+      <c r="F245">
+        <v>7</v>
+      </c>
+      <c r="G245">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="H245" t="s">
+        <v>371</v>
+      </c>
+      <c r="I245">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K245">
+        <f>I245/G245</f>
+        <v>0.19881305637982197</v>
+      </c>
+      <c r="M245">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>366</v>
+      </c>
+      <c r="B246" t="s">
+        <v>367</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D246" t="s">
+        <v>356</v>
+      </c>
+      <c r="E246">
+        <v>4</v>
+      </c>
+      <c r="F246">
+        <v>7</v>
+      </c>
+      <c r="G246">
+        <v>0.39</v>
+      </c>
+      <c r="H246" t="s">
+        <v>372</v>
+      </c>
+      <c r="I246">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="K246">
+        <f>I246/G246</f>
+        <v>0.2282051282051282</v>
+      </c>
+      <c r="M246">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>366</v>
+      </c>
+      <c r="B247" t="s">
+        <v>367</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D247" t="s">
+        <v>356</v>
+      </c>
+      <c r="E247">
+        <v>5</v>
+      </c>
+      <c r="F247">
+        <v>5</v>
+      </c>
+      <c r="G247">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H247" t="s">
+        <v>373</v>
+      </c>
+      <c r="I247">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K247">
+        <f>I247/G247</f>
+        <v>0.21637426900584791</v>
+      </c>
+      <c r="M247">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>366</v>
+      </c>
+      <c r="B248" t="s">
+        <v>367</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D248" t="s">
+        <v>356</v>
+      </c>
+      <c r="E248">
+        <v>6</v>
+      </c>
+      <c r="F248">
+        <v>7</v>
+      </c>
+      <c r="G248">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="H248" t="s">
+        <v>374</v>
+      </c>
+      <c r="I248">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K248">
+        <f>I248/G248</f>
+        <v>0.25280898876404495</v>
+      </c>
+      <c r="M248">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>149</v>
+      </c>
+      <c r="B249" t="s">
+        <v>168</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D249" t="s">
+        <v>349</v>
+      </c>
+      <c r="E249">
+        <v>3</v>
+      </c>
+      <c r="F249">
+        <v>7</v>
+      </c>
+      <c r="G249">
+        <v>0.752</v>
+      </c>
+      <c r="H249" t="s">
+        <v>375</v>
+      </c>
+      <c r="I249">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="K249">
+        <f>I249/G249</f>
+        <v>0.19148936170212766</v>
+      </c>
+      <c r="M249">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>149</v>
+      </c>
+      <c r="B250" t="s">
+        <v>168</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D250" t="s">
+        <v>349</v>
+      </c>
+      <c r="E250">
+        <v>4</v>
+      </c>
+      <c r="F250">
+        <v>5</v>
+      </c>
+      <c r="G250">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H250" t="s">
+        <v>376</v>
+      </c>
+      <c r="I250">
+        <v>0.126</v>
+      </c>
+      <c r="K250">
+        <f>I250/G250</f>
+        <v>0.20487804878048782</v>
+      </c>
+      <c r="M250">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>149</v>
+      </c>
+      <c r="B251" t="s">
+        <v>168</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D251" t="s">
+        <v>349</v>
+      </c>
+      <c r="E251">
+        <v>5</v>
+      </c>
+      <c r="F251">
+        <v>3</v>
+      </c>
+      <c r="G251">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="H251" t="s">
+        <v>377</v>
+      </c>
+      <c r="I251">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K251">
+        <f>I251/G251</f>
+        <v>0.21662468513853902</v>
+      </c>
+      <c r="M251">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>86</v>
+      </c>
+      <c r="B252" t="s">
+        <v>87</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D252" t="s">
+        <v>368</v>
+      </c>
+      <c r="E252">
+        <v>1</v>
+      </c>
+      <c r="F252">
+        <v>7</v>
+      </c>
+      <c r="G252">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="H252" t="s">
+        <v>378</v>
+      </c>
+      <c r="I252">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="K252">
+        <f>I252/G252</f>
+        <v>0.27327935222672067</v>
+      </c>
+      <c r="M252">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>86</v>
+      </c>
+      <c r="B253" t="s">
+        <v>87</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D253" t="s">
+        <v>368</v>
+      </c>
+      <c r="E253">
+        <v>2</v>
+      </c>
+      <c r="F253">
+        <v>5</v>
+      </c>
+      <c r="G253">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="H253" t="s">
+        <v>379</v>
+      </c>
+      <c r="I253">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="K253">
+        <f>I253/G253</f>
+        <v>0.26427406199021208</v>
+      </c>
+      <c r="M253">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>86</v>
+      </c>
+      <c r="B254" t="s">
+        <v>87</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D254" t="s">
+        <v>368</v>
+      </c>
+      <c r="E254">
+        <v>3</v>
+      </c>
+      <c r="F254">
+        <v>5</v>
+      </c>
+      <c r="G254">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="H254" t="s">
+        <v>380</v>
+      </c>
+      <c r="I254">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="K254">
+        <f>I254/G254</f>
+        <v>0.25268817204301069</v>
+      </c>
+      <c r="M254">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>86</v>
+      </c>
+      <c r="B255" t="s">
+        <v>87</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D255" t="s">
+        <v>368</v>
+      </c>
+      <c r="E255">
+        <v>4</v>
+      </c>
+      <c r="F255">
+        <v>5</v>
+      </c>
+      <c r="G255">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="H255" t="s">
+        <v>381</v>
+      </c>
+      <c r="I255">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="K255">
+        <f>I255/G255</f>
+        <v>0.25192012288786481</v>
+      </c>
+      <c r="M255">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>86</v>
+      </c>
+      <c r="B256" t="s">
+        <v>87</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D256" t="s">
+        <v>368</v>
+      </c>
+      <c r="E256">
+        <v>5</v>
+      </c>
+      <c r="F256">
+        <v>5</v>
+      </c>
+      <c r="G256">
+        <v>0.379</v>
+      </c>
+      <c r="H256" t="s">
+        <v>382</v>
+      </c>
+      <c r="I256">
+        <v>0.107</v>
+      </c>
+      <c r="K256">
+        <f>I256/G256</f>
+        <v>0.28232189973614774</v>
+      </c>
+      <c r="M256">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>383</v>
+      </c>
+      <c r="B257" t="s">
+        <v>384</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D257" t="s">
+        <v>368</v>
+      </c>
+      <c r="E257">
+        <v>1</v>
+      </c>
+      <c r="F257">
+        <v>5</v>
+      </c>
+      <c r="G257">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="H257" t="s">
+        <v>385</v>
+      </c>
+      <c r="I257">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="K257">
+        <f>I257/G257</f>
+        <v>0.25874125874125875</v>
+      </c>
+      <c r="M257">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>383</v>
+      </c>
+      <c r="B258" t="s">
+        <v>384</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D258" t="s">
+        <v>368</v>
+      </c>
+      <c r="E258">
+        <v>2</v>
+      </c>
+      <c r="F258">
+        <v>5</v>
+      </c>
+      <c r="G258">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="H258" t="s">
+        <v>386</v>
+      </c>
+      <c r="I258">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K258">
+        <f>I258/G258</f>
+        <v>0.2087591240875912</v>
+      </c>
+      <c r="M258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>383</v>
+      </c>
+      <c r="B259" t="s">
+        <v>384</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D259" t="s">
+        <v>368</v>
+      </c>
+      <c r="E259">
+        <v>3</v>
+      </c>
+      <c r="F259">
+        <v>4</v>
+      </c>
+      <c r="G259">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="H259" t="s">
+        <v>387</v>
+      </c>
+      <c r="I259">
+        <v>0.185</v>
+      </c>
+      <c r="K259">
+        <f>I259/G259</f>
+        <v>0.27903469079939669</v>
+      </c>
+      <c r="M259">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>383</v>
+      </c>
+      <c r="B260" t="s">
+        <v>384</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D260" t="s">
+        <v>368</v>
+      </c>
+      <c r="E260">
+        <v>4</v>
+      </c>
+      <c r="F260">
+        <v>5</v>
+      </c>
+      <c r="G260">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="H260" t="s">
+        <v>388</v>
+      </c>
+      <c r="I260">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="K260">
+        <f>I260/G260</f>
+        <v>0.32334384858044163</v>
+      </c>
+      <c r="M260">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>383</v>
+      </c>
+      <c r="B261" t="s">
+        <v>384</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D261" t="s">
+        <v>368</v>
+      </c>
+      <c r="E261">
+        <v>5</v>
+      </c>
+      <c r="F261">
+        <v>5</v>
+      </c>
+      <c r="G261">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="H261" t="s">
+        <v>389</v>
+      </c>
+      <c r="I261">
+        <v>0.246</v>
+      </c>
+      <c r="K261">
+        <f>I261/G261</f>
+        <v>0.27003293084522501</v>
+      </c>
+      <c r="M261">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>144</v>
+      </c>
+      <c r="B262" t="s">
+        <v>145</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D262" t="s">
+        <v>349</v>
+      </c>
+      <c r="E262">
+        <v>1</v>
+      </c>
+      <c r="F262">
+        <v>5</v>
+      </c>
+      <c r="G262">
+        <v>3.0289999999999999</v>
+      </c>
+      <c r="H262" t="s">
+        <v>390</v>
+      </c>
+      <c r="I262">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="K262">
+        <f>I262/G262</f>
+        <v>0.13007593265103995</v>
+      </c>
+      <c r="M262">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>144</v>
+      </c>
+      <c r="B263" t="s">
+        <v>145</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D263" t="s">
+        <v>349</v>
+      </c>
+      <c r="E263">
+        <v>2</v>
+      </c>
+      <c r="F263">
+        <v>4</v>
+      </c>
+      <c r="G263">
+        <v>1.738</v>
+      </c>
+      <c r="H263" t="s">
+        <v>391</v>
+      </c>
+      <c r="I263">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="K263">
+        <f>I263/G263</f>
+        <v>0.11967779056386652</v>
+      </c>
+      <c r="M263">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>144</v>
+      </c>
+      <c r="B264" t="s">
+        <v>145</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D264" t="s">
+        <v>349</v>
+      </c>
+      <c r="E264">
+        <v>3</v>
+      </c>
+      <c r="F264">
+        <v>5</v>
+      </c>
+      <c r="G264">
+        <v>2.863</v>
+      </c>
+      <c r="H264" t="s">
+        <v>392</v>
+      </c>
+      <c r="I264">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="K264">
+        <f>I264/G264</f>
+        <v>0.13796716730702061</v>
+      </c>
+      <c r="M264">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>144</v>
+      </c>
+      <c r="B265" t="s">
+        <v>145</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D265" t="s">
+        <v>349</v>
+      </c>
+      <c r="E265">
+        <v>4</v>
+      </c>
+      <c r="F265">
+        <v>5</v>
+      </c>
+      <c r="G265">
+        <v>3.5230000000000001</v>
+      </c>
+      <c r="H265" t="s">
+        <v>393</v>
+      </c>
+      <c r="I265">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="K265">
+        <f>I265/G265</f>
+        <v>0.12688049957422651</v>
+      </c>
+      <c r="M265">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>144</v>
+      </c>
+      <c r="B266" t="s">
+        <v>145</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D266" t="s">
+        <v>349</v>
+      </c>
+      <c r="E266">
+        <v>5</v>
+      </c>
+      <c r="F266">
+        <v>6</v>
+      </c>
+      <c r="G266">
+        <v>5.3780000000000001</v>
+      </c>
+      <c r="H266" t="s">
+        <v>394</v>
+      </c>
+      <c r="I266">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="J266" t="s">
+        <v>395</v>
+      </c>
+      <c r="K266">
+        <f>I266/G266</f>
+        <v>0.10710301227222015</v>
+      </c>
+      <c r="M266">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>396</v>
+      </c>
+      <c r="B267" t="s">
+        <v>397</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D267" t="s">
+        <v>349</v>
+      </c>
+      <c r="E267">
+        <v>1</v>
+      </c>
+      <c r="F267">
+        <v>7</v>
+      </c>
+      <c r="G267">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H267" t="s">
+        <v>398</v>
+      </c>
+      <c r="I267">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K267">
+        <f>I267/G267</f>
+        <v>0.17938144329896907</v>
+      </c>
+      <c r="M267">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>396</v>
+      </c>
+      <c r="B268" t="s">
+        <v>397</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D268" t="s">
+        <v>349</v>
+      </c>
+      <c r="E268">
+        <v>2</v>
+      </c>
+      <c r="F268">
+        <v>7</v>
+      </c>
+      <c r="G268">
+        <v>0.217</v>
+      </c>
+      <c r="H268" t="s">
+        <v>399</v>
+      </c>
+      <c r="I268">
+        <v>3.1E-2</v>
+      </c>
+      <c r="K268">
+        <f>I268/G268</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="M268">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>396</v>
+      </c>
+      <c r="B269" t="s">
+        <v>397</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D269" t="s">
+        <v>349</v>
+      </c>
+      <c r="E269">
+        <v>3</v>
+      </c>
+      <c r="F269">
+        <v>7</v>
+      </c>
+      <c r="G269">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="H269" t="s">
+        <v>400</v>
+      </c>
+      <c r="I269">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K269">
+        <f>I269/G269</f>
+        <v>0.18497109826589597</v>
+      </c>
+      <c r="M269">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>396</v>
+      </c>
+      <c r="B270" t="s">
+        <v>397</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D270" t="s">
+        <v>349</v>
+      </c>
+      <c r="E270">
+        <v>4</v>
+      </c>
+      <c r="F270">
+        <v>7</v>
+      </c>
+      <c r="G270">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="H270" t="s">
+        <v>401</v>
+      </c>
+      <c r="I270">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="K270">
+        <f>I270/G270</f>
+        <v>0.18067226890756302</v>
+      </c>
+      <c r="M270">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>396</v>
+      </c>
+      <c r="B271" t="s">
+        <v>397</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D271" t="s">
+        <v>349</v>
+      </c>
+      <c r="E271">
+        <v>5</v>
+      </c>
+      <c r="F271">
+        <v>6</v>
+      </c>
+      <c r="G271">
+        <v>0.309</v>
+      </c>
+      <c r="H271" t="s">
+        <v>402</v>
+      </c>
+      <c r="I271">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K271">
+        <f>I271/G271</f>
+        <v>0.15533980582524273</v>
+      </c>
+      <c r="M271">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>396</v>
+      </c>
+      <c r="B272" t="s">
+        <v>397</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D272" t="s">
+        <v>349</v>
+      </c>
+      <c r="E272">
+        <v>6</v>
+      </c>
+      <c r="F272">
+        <v>7</v>
+      </c>
+      <c r="G272">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="H272" t="s">
+        <v>403</v>
+      </c>
+      <c r="I272">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K272">
+        <f>I272/G272</f>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="M272">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>396</v>
+      </c>
+      <c r="B273" t="s">
+        <v>397</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D273" t="s">
+        <v>349</v>
+      </c>
+      <c r="E273">
+        <v>7</v>
+      </c>
+      <c r="F273">
+        <v>7</v>
+      </c>
+      <c r="G273">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="H273" t="s">
+        <v>404</v>
+      </c>
+      <c r="I273">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="K273">
+        <f>I273/G273</f>
+        <v>0.16804407713498623</v>
+      </c>
+      <c r="M273">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>316</v>
+      </c>
+      <c r="B274" t="s">
+        <v>317</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D274" t="s">
+        <v>349</v>
+      </c>
+      <c r="E274">
+        <v>1</v>
+      </c>
+      <c r="F274">
+        <v>5</v>
+      </c>
+      <c r="G274">
+        <v>2.3879999999999999</v>
+      </c>
+      <c r="H274" t="s">
+        <v>405</v>
+      </c>
+      <c r="I274">
+        <v>0.33</v>
+      </c>
+      <c r="K274">
+        <f>I274/G274</f>
+        <v>0.13819095477386936</v>
+      </c>
+      <c r="M274">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>316</v>
+      </c>
+      <c r="B275" t="s">
+        <v>317</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D275" t="s">
+        <v>349</v>
+      </c>
+      <c r="E275">
+        <v>2</v>
+      </c>
+      <c r="F275">
+        <v>5</v>
+      </c>
+      <c r="G275">
+        <v>1.6</v>
+      </c>
+      <c r="H275" t="s">
+        <v>406</v>
+      </c>
+      <c r="I275">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="K275">
+        <f>I275/G275</f>
+        <v>0.13062499999999999</v>
+      </c>
+      <c r="M275">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>316</v>
+      </c>
+      <c r="B276" t="s">
+        <v>317</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D276" t="s">
+        <v>349</v>
+      </c>
+      <c r="E276">
+        <v>3</v>
+      </c>
+      <c r="F276">
+        <v>3</v>
+      </c>
+      <c r="G276">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="H276" t="s">
+        <v>407</v>
+      </c>
+      <c r="I276">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="K276">
+        <f>I276/G276</f>
+        <v>0.12740384615384615</v>
+      </c>
+      <c r="M276">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>316</v>
+      </c>
+      <c r="B277" t="s">
+        <v>317</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D277" t="s">
+        <v>349</v>
+      </c>
+      <c r="E277">
+        <v>4</v>
+      </c>
+      <c r="F277">
+        <v>4</v>
+      </c>
+      <c r="G277">
+        <v>4.54</v>
+      </c>
+      <c r="H277" t="s">
+        <v>408</v>
+      </c>
+      <c r="I277">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="K277">
+        <f>I277/G277</f>
+        <v>0.12466960352422907</v>
+      </c>
+      <c r="M277">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>316</v>
+      </c>
+      <c r="B278" t="s">
+        <v>317</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D278" t="s">
+        <v>349</v>
+      </c>
+      <c r="E278">
+        <v>5</v>
+      </c>
+      <c r="F278">
+        <v>6</v>
+      </c>
+      <c r="G278">
+        <v>6.6509999999999998</v>
+      </c>
+      <c r="H278" t="s">
+        <v>409</v>
+      </c>
+      <c r="I278">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="J278" t="s">
+        <v>410</v>
+      </c>
+      <c r="K278">
+        <f>I278/G278</f>
+        <v>0.13351375732972487</v>
+      </c>
+      <c r="M278">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>411</v>
+      </c>
+      <c r="B279" t="s">
+        <v>412</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D279" t="s">
+        <v>349</v>
+      </c>
+      <c r="E279">
+        <v>1</v>
+      </c>
+      <c r="F279">
+        <v>5</v>
+      </c>
+      <c r="G279">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="H279" t="s">
+        <v>413</v>
+      </c>
+      <c r="I279">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="K279">
+        <f>I279/G279</f>
+        <v>0.23753665689149558</v>
+      </c>
+      <c r="M279">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>411</v>
+      </c>
+      <c r="B280" t="s">
+        <v>412</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D280" t="s">
+        <v>349</v>
+      </c>
+      <c r="E280">
+        <v>2</v>
+      </c>
+      <c r="F280">
+        <v>5</v>
+      </c>
+      <c r="G280">
+        <v>1.482</v>
+      </c>
+      <c r="H280" t="s">
+        <v>415</v>
+      </c>
+      <c r="I280">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="K280">
+        <f>I280/G280</f>
+        <v>0.2213225371120108</v>
+      </c>
+      <c r="M280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>411</v>
+      </c>
+      <c r="B281" t="s">
+        <v>412</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D281" t="s">
+        <v>349</v>
+      </c>
+      <c r="E281">
+        <v>3</v>
+      </c>
+      <c r="F281">
+        <v>4</v>
+      </c>
+      <c r="G281">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="H281" t="s">
+        <v>414</v>
+      </c>
+      <c r="I281">
+        <v>0.156</v>
+      </c>
+      <c r="K281">
+        <f>I281/G281</f>
+        <v>0.22096317280453259</v>
+      </c>
+      <c r="M281">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>411</v>
+      </c>
+      <c r="B282" t="s">
+        <v>412</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D282" t="s">
+        <v>349</v>
+      </c>
+      <c r="E282">
+        <v>4</v>
+      </c>
+      <c r="F282">
+        <v>5</v>
+      </c>
+      <c r="G282">
+        <v>1.571</v>
+      </c>
+      <c r="H282" t="s">
+        <v>416</v>
+      </c>
+      <c r="I282">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="K282">
+        <f>I282/G282</f>
+        <v>0.23042647994907703</v>
+      </c>
+      <c r="M282">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>29</v>
+      </c>
+      <c r="B283" t="s">
+        <v>417</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D283" t="s">
+        <v>349</v>
+      </c>
+      <c r="E283">
+        <v>1</v>
+      </c>
+      <c r="F283">
+        <v>7</v>
+      </c>
+      <c r="G283">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="H283" t="s">
+        <v>418</v>
+      </c>
+      <c r="I283">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="K283">
+        <f>I283/G283</f>
+        <v>0.36538461538461542</v>
+      </c>
+      <c r="M283">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>29</v>
+      </c>
+      <c r="B284" t="s">
+        <v>417</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D284" t="s">
+        <v>349</v>
+      </c>
+      <c r="E284">
+        <v>2</v>
+      </c>
+      <c r="F284">
+        <v>7</v>
+      </c>
+      <c r="G284">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="H284" t="s">
+        <v>419</v>
+      </c>
+      <c r="I284">
+        <v>0.124</v>
+      </c>
+      <c r="K284">
+        <f>I284/G284</f>
+        <v>0.33787465940054495</v>
+      </c>
+      <c r="M284">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>29</v>
+      </c>
+      <c r="B285" t="s">
+        <v>417</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D285" t="s">
+        <v>349</v>
+      </c>
+      <c r="E285">
+        <v>3</v>
+      </c>
+      <c r="F285">
+        <v>7</v>
+      </c>
+      <c r="G285">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H285" t="s">
+        <v>420</v>
+      </c>
+      <c r="I285">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K285">
+        <f>I285/G285</f>
+        <v>0.29531568228105903</v>
+      </c>
+      <c r="M285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>29</v>
+      </c>
+      <c r="B286" t="s">
+        <v>417</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D286" t="s">
+        <v>349</v>
+      </c>
+      <c r="E286">
+        <v>4</v>
+      </c>
+      <c r="F286">
+        <v>6</v>
+      </c>
+      <c r="G286">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="H286" t="s">
+        <v>421</v>
+      </c>
+      <c r="I286">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K286">
+        <f>I286/G286</f>
+        <v>0.28937728937728935</v>
+      </c>
+      <c r="M286">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>25</v>
+      </c>
+      <c r="B287" t="s">
+        <v>26</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D287" t="s">
+        <v>349</v>
+      </c>
+      <c r="E287">
+        <v>1</v>
+      </c>
+      <c r="F287">
+        <v>7</v>
+      </c>
+      <c r="G287">
+        <v>1.427</v>
+      </c>
+      <c r="H287" t="s">
+        <v>422</v>
+      </c>
+      <c r="I287">
+        <v>0.373</v>
+      </c>
+      <c r="K287">
+        <f>I287/G287</f>
+        <v>0.26138752627890677</v>
+      </c>
+      <c r="M287">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>25</v>
+      </c>
+      <c r="B288" t="s">
+        <v>26</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D288" t="s">
+        <v>349</v>
+      </c>
+      <c r="E288">
+        <v>2</v>
+      </c>
+      <c r="F288">
+        <v>5</v>
+      </c>
+      <c r="G288">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="H288" t="s">
+        <v>423</v>
+      </c>
+      <c r="I288">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="K288">
+        <f>I288/G288</f>
+        <v>0.3378076062639821</v>
+      </c>
+      <c r="M288">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>25</v>
+      </c>
+      <c r="B289" t="s">
+        <v>26</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D289" t="s">
+        <v>349</v>
+      </c>
+      <c r="E289">
+        <v>3</v>
+      </c>
+      <c r="F289">
+        <v>4</v>
+      </c>
+      <c r="G289">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="H289" t="s">
+        <v>424</v>
+      </c>
+      <c r="I289">
+        <v>0.17</v>
+      </c>
+      <c r="K289">
+        <f>I289/G289</f>
+        <v>0.24566473988439311</v>
+      </c>
+      <c r="M289">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>25</v>
+      </c>
+      <c r="B290" t="s">
+        <v>26</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D290" t="s">
+        <v>349</v>
+      </c>
+      <c r="E290">
+        <v>4</v>
+      </c>
+      <c r="F290">
+        <v>3</v>
+      </c>
+      <c r="G290">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H290" t="s">
+        <v>425</v>
+      </c>
+      <c r="I290">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K290">
+        <f>I290/G290</f>
+        <v>0.23868312757201648</v>
+      </c>
+      <c r="M290">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>25</v>
+      </c>
+      <c r="B291" t="s">
+        <v>26</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D291" t="s">
+        <v>349</v>
+      </c>
+      <c r="E291">
+        <v>5</v>
+      </c>
+      <c r="F291">
+        <v>3</v>
+      </c>
+      <c r="G291">
+        <v>0.434</v>
+      </c>
+      <c r="H291" t="s">
+        <v>426</v>
+      </c>
+      <c r="I291">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K291">
+        <f>I291/G291</f>
+        <v>0.32949308755760365</v>
+      </c>
+      <c r="M291">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added table of total leaf areas per scan.
</commit_message>
<xml_diff>
--- a/Files/Trait data.xlsx
+++ b/Files/Trait data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PhD\Travels\Euskal_fd\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD8F8DB-E97B-42B1-8085-9E8D69E4F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0271B913-5668-49AE-A967-7B370331902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="448">
   <si>
     <t>Genus</t>
   </si>
@@ -1318,6 +1318,69 @@
   </si>
   <si>
     <t>G056</t>
+  </si>
+  <si>
+    <t>rupestre</t>
+  </si>
+  <si>
+    <t>17.07.</t>
+  </si>
+  <si>
+    <t>ORGI1</t>
+  </si>
+  <si>
+    <t>H001</t>
+  </si>
+  <si>
+    <t>H002</t>
+  </si>
+  <si>
+    <t>H003</t>
+  </si>
+  <si>
+    <t>H004</t>
+  </si>
+  <si>
+    <t>H005</t>
+  </si>
+  <si>
+    <t>H006</t>
+  </si>
+  <si>
+    <t>H007</t>
+  </si>
+  <si>
+    <t>H008</t>
+  </si>
+  <si>
+    <t>H009</t>
+  </si>
+  <si>
+    <t>officinalis</t>
+  </si>
+  <si>
+    <t>H010</t>
+  </si>
+  <si>
+    <t>H011</t>
+  </si>
+  <si>
+    <t>H012</t>
+  </si>
+  <si>
+    <t>H013</t>
+  </si>
+  <si>
+    <t>H014</t>
+  </si>
+  <si>
+    <t>H015</t>
+  </si>
+  <si>
+    <t>H016</t>
+  </si>
+  <si>
+    <t>H017</t>
   </si>
 </sst>
 </file>
@@ -1678,11 +1741,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M291"/>
+  <dimension ref="A1:M308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q301" sqref="Q301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,7 +1827,7 @@
         <v>0.122</v>
       </c>
       <c r="K2">
-        <f>I2/G2</f>
+        <f t="shared" ref="K2:K65" si="0">I2/G2</f>
         <v>0.15307402760351316</v>
       </c>
       <c r="M2">
@@ -1800,7 +1863,7 @@
         <v>0.23499999999999999</v>
       </c>
       <c r="K3">
-        <f>I3/G3</f>
+        <f t="shared" si="0"/>
         <v>0.12252346193952034</v>
       </c>
       <c r="M3">
@@ -1836,7 +1899,7 @@
         <v>0.04</v>
       </c>
       <c r="K4">
-        <f>I4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.14869888475836432</v>
       </c>
       <c r="M4">
@@ -1872,7 +1935,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="K5">
-        <f>I5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.16058394160583939</v>
       </c>
       <c r="M5">
@@ -1908,7 +1971,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K6">
-        <f>I6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.1404494382022472</v>
       </c>
       <c r="M6">
@@ -1944,7 +2007,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K7">
-        <f>I7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.15617715617715619</v>
       </c>
       <c r="M7">
@@ -1980,7 +2043,7 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="K8">
-        <f>I8/G8</f>
+        <f t="shared" si="0"/>
         <v>8.5558931712777869E-2</v>
       </c>
       <c r="M8">
@@ -2016,7 +2079,7 @@
         <v>0.376</v>
       </c>
       <c r="K9">
-        <f>I9/G9</f>
+        <f t="shared" si="0"/>
         <v>0.39788359788359789</v>
       </c>
       <c r="M9">
@@ -2052,7 +2115,7 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="K10">
-        <f>I10/G10</f>
+        <f t="shared" si="0"/>
         <v>0.41915227629513346</v>
       </c>
       <c r="M10">
@@ -2088,7 +2151,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K11">
-        <f>I11/G11</f>
+        <f t="shared" si="0"/>
         <v>0.27756653992395436</v>
       </c>
       <c r="M11">
@@ -2124,7 +2187,7 @@
         <v>6.3E-2</v>
       </c>
       <c r="K12">
-        <f>I12/G12</f>
+        <f t="shared" si="0"/>
         <v>0.24230769230769231</v>
       </c>
       <c r="M12">
@@ -2160,7 +2223,7 @@
         <v>6.3E-2</v>
       </c>
       <c r="K13">
-        <f>I13/G13</f>
+        <f t="shared" si="0"/>
         <v>0.21501706484641639</v>
       </c>
       <c r="M13">
@@ -2196,7 +2259,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="K14">
-        <f>I14/G14</f>
+        <f t="shared" si="0"/>
         <v>0.22950819672131148</v>
       </c>
       <c r="M14">
@@ -2232,7 +2295,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="K15">
-        <f>I15/G15</f>
+        <f t="shared" si="0"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="M15">
@@ -2268,7 +2331,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K16">
-        <f>I16/G16</f>
+        <f t="shared" si="0"/>
         <v>0.21739130434782608</v>
       </c>
       <c r="M16">
@@ -2304,7 +2367,7 @@
         <v>0.47599999999999998</v>
       </c>
       <c r="K17">
-        <f>I17/G17</f>
+        <f t="shared" si="0"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="M17">
@@ -2340,7 +2403,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="K18">
-        <f>I18/G18</f>
+        <f t="shared" si="0"/>
         <v>0.27569331158238175</v>
       </c>
       <c r="M18">
@@ -2376,7 +2439,7 @@
         <v>0.36699999999999999</v>
       </c>
       <c r="K19">
-        <f>I19/G19</f>
+        <f t="shared" si="0"/>
         <v>0.25051194539249144</v>
       </c>
       <c r="M19">
@@ -2412,7 +2475,7 @@
         <v>0.189</v>
       </c>
       <c r="K20">
-        <f>I20/G20</f>
+        <f t="shared" si="0"/>
         <v>0.29032258064516125</v>
       </c>
       <c r="M20">
@@ -2448,7 +2511,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="K21">
-        <f>I21/G21</f>
+        <f t="shared" si="0"/>
         <v>0.21188630490956073</v>
       </c>
       <c r="M21">
@@ -2484,7 +2547,7 @@
         <v>0.124</v>
       </c>
       <c r="K22">
-        <f>I22/G22</f>
+        <f t="shared" si="0"/>
         <v>0.40522875816993464</v>
       </c>
       <c r="M22">
@@ -2520,7 +2583,7 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="K23">
-        <f>I23/G23</f>
+        <f t="shared" si="0"/>
         <v>0.17229129662522205</v>
       </c>
       <c r="M23">
@@ -2556,7 +2619,7 @@
         <v>0.24</v>
       </c>
       <c r="K24">
-        <f>I24/G24</f>
+        <f t="shared" si="0"/>
         <v>0.13392857142857142</v>
       </c>
       <c r="M24">
@@ -2592,7 +2655,7 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="K25">
-        <f>I25/G25</f>
+        <f t="shared" si="0"/>
         <v>0.15053091817613992</v>
       </c>
       <c r="M25">
@@ -2628,7 +2691,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="K26">
-        <f>I26/G26</f>
+        <f t="shared" si="0"/>
         <v>0.34635416666666669</v>
       </c>
       <c r="M26">
@@ -2664,7 +2727,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="K27">
-        <f>I27/G27</f>
+        <f t="shared" si="0"/>
         <v>0.36818181818181817</v>
       </c>
       <c r="M27">
@@ -2700,7 +2763,7 @@
         <v>0.111</v>
       </c>
       <c r="K28">
-        <f>I28/G28</f>
+        <f t="shared" si="0"/>
         <v>0.36513157894736842</v>
       </c>
       <c r="M28">
@@ -2736,7 +2799,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="K29">
-        <f>I29/G29</f>
+        <f t="shared" si="0"/>
         <v>0.10144927536231883</v>
       </c>
       <c r="M29">
@@ -2772,7 +2835,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="K30">
-        <f>I30/G30</f>
+        <f t="shared" si="0"/>
         <v>0.16760828625235402</v>
       </c>
       <c r="M30">
@@ -2808,7 +2871,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K31">
-        <f>I31/G31</f>
+        <f t="shared" si="0"/>
         <v>0.15594855305466238</v>
       </c>
       <c r="M31">
@@ -2844,7 +2907,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="K32">
-        <f>I32/G32</f>
+        <f t="shared" si="0"/>
         <v>0.13809523809523808</v>
       </c>
       <c r="M32">
@@ -2880,7 +2943,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="K33">
-        <f>I33/G33</f>
+        <f t="shared" si="0"/>
         <v>0.2299465240641711</v>
       </c>
       <c r="M33">
@@ -2916,7 +2979,7 @@
         <v>0.186</v>
       </c>
       <c r="K34">
-        <f>I34/G34</f>
+        <f t="shared" si="0"/>
         <v>0.25340599455040874</v>
       </c>
       <c r="M34">
@@ -2952,7 +3015,7 @@
         <v>0.155</v>
       </c>
       <c r="K35">
-        <f>I35/G35</f>
+        <f t="shared" si="0"/>
         <v>0.22794117647058823</v>
       </c>
       <c r="M35">
@@ -2988,7 +3051,7 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="K36">
-        <f>I36/G36</f>
+        <f t="shared" si="0"/>
         <v>0.26106526631657911</v>
       </c>
       <c r="M36">
@@ -3024,7 +3087,7 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="K37">
-        <f>I37/G37</f>
+        <f t="shared" si="0"/>
         <v>0.11817726589884826</v>
       </c>
       <c r="M37">
@@ -3060,7 +3123,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="K38">
-        <f>I38/G38</f>
+        <f t="shared" si="0"/>
         <v>0.18032786885245902</v>
       </c>
       <c r="M38">
@@ -3096,7 +3159,7 @@
         <v>0.27300000000000002</v>
       </c>
       <c r="K39">
-        <f>I39/G39</f>
+        <f t="shared" si="0"/>
         <v>0.2426666666666667</v>
       </c>
       <c r="M39">
@@ -3132,7 +3195,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="K40">
-        <f>I40/G40</f>
+        <f t="shared" si="0"/>
         <v>0.13983050847457629</v>
       </c>
       <c r="M40">
@@ -3165,7 +3228,7 @@
         <v>0.05</v>
       </c>
       <c r="K41">
-        <f>I41/G41</f>
+        <f t="shared" si="0"/>
         <v>0.43859649122807021</v>
       </c>
       <c r="L41" t="s">
@@ -3204,7 +3267,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K42">
-        <f>I42/G42</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="M42">
@@ -3240,7 +3303,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K43">
-        <f>I43/G43</f>
+        <f t="shared" si="0"/>
         <v>0.33500000000000002</v>
       </c>
       <c r="M43">
@@ -3276,7 +3339,7 @@
         <v>0.128</v>
       </c>
       <c r="K44">
-        <f>I44/G44</f>
+        <f t="shared" si="0"/>
         <v>0.32569974554707376</v>
       </c>
       <c r="M44">
@@ -3312,7 +3375,7 @@
         <v>0.66800000000000004</v>
       </c>
       <c r="K45">
-        <f>I45/G45</f>
+        <f t="shared" si="0"/>
         <v>7.6030047803323481E-2</v>
       </c>
       <c r="M45">
@@ -3348,7 +3411,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K46">
-        <f>I46/G46</f>
+        <f t="shared" si="0"/>
         <v>7.5952693823915896E-2</v>
       </c>
       <c r="M46">
@@ -3384,7 +3447,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K47">
-        <f>I47/G47</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="M47">
@@ -3420,7 +3483,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K48">
-        <f>I48/G48</f>
+        <f t="shared" si="0"/>
         <v>0.17156862745098037</v>
       </c>
       <c r="M48">
@@ -3456,7 +3519,7 @@
         <v>0.224</v>
       </c>
       <c r="K49">
-        <f>I49/G49</f>
+        <f t="shared" si="0"/>
         <v>0.15774647887323945</v>
       </c>
       <c r="M49">
@@ -3492,7 +3555,7 @@
         <v>0.36799999999999999</v>
       </c>
       <c r="K50">
-        <f>I50/G50</f>
+        <f t="shared" si="0"/>
         <v>0.16211453744493393</v>
       </c>
       <c r="M50">
@@ -3531,7 +3594,7 @@
         <v>104</v>
       </c>
       <c r="K51">
-        <f>I51/G51</f>
+        <f t="shared" si="0"/>
         <v>0.18175338560228083</v>
       </c>
       <c r="M51">
@@ -3570,7 +3633,7 @@
         <v>106</v>
       </c>
       <c r="K52">
-        <f>I52/G52</f>
+        <f t="shared" si="0"/>
         <v>0.16235427921524026</v>
       </c>
       <c r="M52">
@@ -3606,7 +3669,7 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="K53">
-        <f>I53/G53</f>
+        <f t="shared" si="0"/>
         <v>0.14320154291224688</v>
       </c>
       <c r="M53">
@@ -3642,7 +3705,7 @@
         <v>0.33400000000000002</v>
       </c>
       <c r="K54">
-        <f>I54/G54</f>
+        <f t="shared" si="0"/>
         <v>0.13813068651778329</v>
       </c>
       <c r="M54">
@@ -3678,7 +3741,7 @@
         <v>0.112</v>
       </c>
       <c r="K55">
-        <f>I55/G55</f>
+        <f t="shared" si="0"/>
         <v>0.1761006289308176</v>
       </c>
       <c r="M55">
@@ -3714,7 +3777,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="K56">
-        <f>I56/G56</f>
+        <f t="shared" si="0"/>
         <v>0.29273285568065505</v>
       </c>
       <c r="M56">
@@ -3750,7 +3813,7 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="K57">
-        <f>I57/G57</f>
+        <f t="shared" si="0"/>
         <v>0.1603960396039604</v>
       </c>
       <c r="M57">
@@ -3786,7 +3849,7 @@
         <v>0.127</v>
       </c>
       <c r="K58">
-        <f>I58/G58</f>
+        <f t="shared" si="0"/>
         <v>0.15855181023720349</v>
       </c>
       <c r="L58" t="s">
@@ -3825,7 +3888,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K59">
-        <f>I59/G59</f>
+        <f t="shared" si="0"/>
         <v>0.15204678362573099</v>
       </c>
       <c r="M59">
@@ -3861,7 +3924,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="K60">
-        <f>I60/G60</f>
+        <f t="shared" si="0"/>
         <v>0.14537444933920704</v>
       </c>
       <c r="M60">
@@ -3897,7 +3960,7 @@
         <v>0.08</v>
       </c>
       <c r="K61">
-        <f>I61/G61</f>
+        <f t="shared" si="0"/>
         <v>0.14234875444839856</v>
       </c>
       <c r="M61">
@@ -3933,7 +3996,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="K62">
-        <f>I62/G62</f>
+        <f t="shared" si="0"/>
         <v>0.13892709766162312</v>
       </c>
       <c r="M62">
@@ -3969,7 +4032,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="K63">
-        <f>I63/G63</f>
+        <f t="shared" si="0"/>
         <v>0.1966292134831461</v>
       </c>
       <c r="M63">
@@ -4005,7 +4068,7 @@
         <v>0.499</v>
       </c>
       <c r="K64">
-        <f>I64/G64</f>
+        <f t="shared" si="0"/>
         <v>0.13652530779753763</v>
       </c>
       <c r="M64">
@@ -4041,7 +4104,7 @@
         <v>0.33500000000000002</v>
       </c>
       <c r="K65">
-        <f>I65/G65</f>
+        <f t="shared" si="0"/>
         <v>0.14093395035759362</v>
       </c>
       <c r="M65">
@@ -4077,7 +4140,7 @@
         <v>0.85799999999999998</v>
       </c>
       <c r="K66">
-        <f>I66/G66</f>
+        <f t="shared" ref="K66:K129" si="1">I66/G66</f>
         <v>0.14415322580645162</v>
       </c>
       <c r="M66">
@@ -4113,7 +4176,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="K67">
-        <f>I67/G67</f>
+        <f t="shared" si="1"/>
         <v>0.11951364175563466</v>
       </c>
       <c r="M67">
@@ -4149,7 +4212,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K68">
-        <f>I68/G68</f>
+        <f t="shared" si="1"/>
         <v>0.18384615384615383</v>
       </c>
       <c r="M68">
@@ -4185,7 +4248,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="K69">
-        <f>I69/G69</f>
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="M69">
@@ -4221,7 +4284,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="K70">
-        <f>I70/G70</f>
+        <f t="shared" si="1"/>
         <v>0.12992125984251968</v>
       </c>
       <c r="M70">
@@ -4257,7 +4320,7 @@
         <v>0.307</v>
       </c>
       <c r="K71">
-        <f>I71/G71</f>
+        <f t="shared" si="1"/>
         <v>0.15258449304174951</v>
       </c>
       <c r="M71">
@@ -4293,7 +4356,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="K72">
-        <f>I72/G72</f>
+        <f t="shared" si="1"/>
         <v>0.15264797507788161</v>
       </c>
       <c r="M72">
@@ -4329,7 +4392,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="K73">
-        <f>I73/G73</f>
+        <f t="shared" si="1"/>
         <v>0.16569200779727097</v>
       </c>
       <c r="M73">
@@ -4365,7 +4428,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="K74">
-        <f>I74/G74</f>
+        <f t="shared" si="1"/>
         <v>0.26865671641791039</v>
       </c>
       <c r="M74">
@@ -4401,7 +4464,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="K75">
-        <f>I75/G75</f>
+        <f t="shared" si="1"/>
         <v>0.27363184079601988</v>
       </c>
       <c r="M75">
@@ -4437,7 +4500,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="K76">
-        <f>I76/G76</f>
+        <f t="shared" si="1"/>
         <v>0.32926829268292679</v>
       </c>
       <c r="M76">
@@ -4473,7 +4536,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="K77">
-        <f>I77/G77</f>
+        <f t="shared" si="1"/>
         <v>0.17596566523605148</v>
       </c>
       <c r="M77">
@@ -4509,7 +4572,7 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="K78">
-        <f>I78/G78</f>
+        <f t="shared" si="1"/>
         <v>0.17747252747252748</v>
       </c>
       <c r="M78">
@@ -4545,7 +4608,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="K79">
-        <f>I79/G79</f>
+        <f t="shared" si="1"/>
         <v>0.15175995383727639</v>
       </c>
       <c r="M79">
@@ -4581,7 +4644,7 @@
         <v>0.112</v>
       </c>
       <c r="K80">
-        <f>I80/G80</f>
+        <f t="shared" si="1"/>
         <v>0.25168539325842698</v>
       </c>
       <c r="M80">
@@ -4617,7 +4680,7 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="K81">
-        <f>I81/G81</f>
+        <f t="shared" si="1"/>
         <v>0.27878211227402472</v>
       </c>
       <c r="M81">
@@ -4653,7 +4716,7 @@
         <v>0.08</v>
       </c>
       <c r="K82">
-        <f>I82/G82</f>
+        <f t="shared" si="1"/>
         <v>0.31746031746031744</v>
       </c>
       <c r="M82">
@@ -4689,7 +4752,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="K83">
-        <f>I83/G83</f>
+        <f t="shared" si="1"/>
         <v>0.21669106881405562</v>
       </c>
       <c r="M83">
@@ -4725,7 +4788,7 @@
         <v>0.623</v>
       </c>
       <c r="K84">
-        <f>I84/G84</f>
+        <f t="shared" si="1"/>
         <v>0.16653301256348568</v>
       </c>
       <c r="M84">
@@ -4761,7 +4824,7 @@
         <v>0.54800000000000004</v>
       </c>
       <c r="K85">
-        <f>I85/G85</f>
+        <f t="shared" si="1"/>
         <v>0.1928898275255192</v>
       </c>
       <c r="M85">
@@ -4797,7 +4860,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="K86">
-        <f>I86/G86</f>
+        <f t="shared" si="1"/>
         <v>0.16371268656716417</v>
       </c>
       <c r="M86">
@@ -4833,7 +4896,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="K87">
-        <f>I87/G87</f>
+        <f t="shared" si="1"/>
         <v>0.2241813602015113</v>
       </c>
       <c r="M87">
@@ -4869,7 +4932,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="K88">
-        <f>I88/G88</f>
+        <f t="shared" si="1"/>
         <v>0.20634920634920634</v>
       </c>
       <c r="M88">
@@ -4905,7 +4968,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="K89">
-        <f>I89/G89</f>
+        <f t="shared" si="1"/>
         <v>0.21495327102803738</v>
       </c>
       <c r="M89">
@@ -4938,7 +5001,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="K90">
-        <f>I90/G90</f>
+        <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
       <c r="L90" t="s">
@@ -4977,7 +5040,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="K91">
-        <f>I91/G91</f>
+        <f t="shared" si="1"/>
         <v>0.3612903225806452</v>
       </c>
       <c r="M91">
@@ -5013,7 +5076,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K92">
-        <f>I92/G92</f>
+        <f t="shared" si="1"/>
         <v>0.25531914893617019</v>
       </c>
       <c r="M92">
@@ -5049,7 +5112,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K93">
-        <f>I93/G93</f>
+        <f t="shared" si="1"/>
         <v>0.2356020942408377</v>
       </c>
       <c r="M93">
@@ -5085,7 +5148,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="K94">
-        <f>I94/G94</f>
+        <f t="shared" si="1"/>
         <v>0.27066115702479343</v>
       </c>
       <c r="M94">
@@ -5121,7 +5184,7 @@
         <v>0.151</v>
       </c>
       <c r="K95">
-        <f>I95/G95</f>
+        <f t="shared" si="1"/>
         <v>0.24512987012987011</v>
       </c>
       <c r="M95">
@@ -5157,7 +5220,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K96">
-        <f>I96/G96</f>
+        <f t="shared" si="1"/>
         <v>0.273394495412844</v>
       </c>
       <c r="M96">
@@ -5193,7 +5256,7 @@
         <v>0.16</v>
       </c>
       <c r="K97">
-        <f>I97/G97</f>
+        <f t="shared" si="1"/>
         <v>0.31872509960159362</v>
       </c>
       <c r="M97">
@@ -5229,7 +5292,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="K98">
-        <f>I98/G98</f>
+        <f t="shared" si="1"/>
         <v>0.23744292237442921</v>
       </c>
       <c r="M98">
@@ -5265,7 +5328,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="K99">
-        <f>I99/G99</f>
+        <f t="shared" si="1"/>
         <v>0.31720430107526876</v>
       </c>
       <c r="M99">
@@ -5301,7 +5364,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K100">
-        <f>I100/G100</f>
+        <f t="shared" si="1"/>
         <v>0.24792013311148087</v>
       </c>
       <c r="M100">
@@ -5337,7 +5400,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="K101">
-        <f>I101/G101</f>
+        <f t="shared" si="1"/>
         <v>0.13229571984435798</v>
       </c>
       <c r="M101">
@@ -5373,7 +5436,7 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="K102">
-        <f>I102/G102</f>
+        <f t="shared" si="1"/>
         <v>0.21663019693654267</v>
       </c>
       <c r="M102">
@@ -5412,7 +5475,7 @@
         <v>181</v>
       </c>
       <c r="K103">
-        <f>I103/G103</f>
+        <f t="shared" si="1"/>
         <v>0.21598977563192273</v>
       </c>
       <c r="M103">
@@ -5451,7 +5514,7 @@
         <v>183</v>
       </c>
       <c r="K104">
-        <f>I104/G104</f>
+        <f t="shared" si="1"/>
         <v>0.23219597550306212</v>
       </c>
       <c r="M104">
@@ -5487,7 +5550,7 @@
         <v>0.156</v>
       </c>
       <c r="K105">
-        <f>I105/G105</f>
+        <f t="shared" si="1"/>
         <v>0.10303830911492734</v>
       </c>
       <c r="M105">
@@ -5523,7 +5586,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="K106">
-        <f>I106/G106</f>
+        <f t="shared" si="1"/>
         <v>9.7142857142857128E-2</v>
       </c>
       <c r="M106">
@@ -5559,7 +5622,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="K107">
-        <f>I107/G107</f>
+        <f t="shared" si="1"/>
         <v>0.35483870967741932</v>
       </c>
       <c r="M107">
@@ -5595,7 +5658,7 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="K108">
-        <f>I108/G108</f>
+        <f t="shared" si="1"/>
         <v>0.16381418092909539</v>
       </c>
       <c r="M108">
@@ -5631,7 +5694,7 @@
         <v>0.188</v>
       </c>
       <c r="K109">
-        <f>I109/G109</f>
+        <f t="shared" si="1"/>
         <v>0.1407185628742515</v>
       </c>
       <c r="M109">
@@ -5667,7 +5730,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="K110">
-        <f>I110/G110</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="M110">
@@ -5703,7 +5766,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="K111">
-        <f>I111/G111</f>
+        <f t="shared" si="1"/>
         <v>0.23008849557522121</v>
       </c>
       <c r="M111">
@@ -5739,7 +5802,7 @@
         <v>0.111</v>
       </c>
       <c r="K112">
-        <f>I112/G112</f>
+        <f t="shared" si="1"/>
         <v>0.22560975609756098</v>
       </c>
       <c r="M112">
@@ -5775,7 +5838,7 @@
         <v>0.35499999999999998</v>
       </c>
       <c r="K113">
-        <f>I113/G113</f>
+        <f t="shared" si="1"/>
         <v>0.13878029710711492</v>
       </c>
       <c r="M113">
@@ -5811,7 +5874,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K114">
-        <f>I114/G114</f>
+        <f t="shared" si="1"/>
         <v>0.14216084484159219</v>
       </c>
       <c r="M114">
@@ -5847,7 +5910,7 @@
         <v>0.248</v>
       </c>
       <c r="K115">
-        <f>I115/G115</f>
+        <f t="shared" si="1"/>
         <v>0.15432482887367766</v>
       </c>
       <c r="M115">
@@ -5883,7 +5946,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="K116">
-        <f>I116/G116</f>
+        <f t="shared" si="1"/>
         <v>0.10258302583025831</v>
       </c>
       <c r="M116">
@@ -5919,7 +5982,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="K117">
-        <f>I117/G117</f>
+        <f t="shared" si="1"/>
         <v>8.6854460093896718E-2</v>
       </c>
       <c r="M117">
@@ -5955,7 +6018,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K118">
-        <f>I118/G118</f>
+        <f t="shared" si="1"/>
         <v>8.3597883597883602E-2</v>
       </c>
       <c r="M118">
@@ -5994,7 +6057,7 @@
         <v>201</v>
       </c>
       <c r="K119">
-        <f>I119/G119</f>
+        <f t="shared" si="1"/>
         <v>0.19229638341664218</v>
       </c>
       <c r="M119">
@@ -6030,7 +6093,7 @@
         <v>0.155</v>
       </c>
       <c r="K120">
-        <f>I120/G120</f>
+        <f t="shared" si="1"/>
         <v>0.16028955532574973</v>
       </c>
       <c r="M120">
@@ -6066,7 +6129,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="K121">
-        <f>I121/G121</f>
+        <f t="shared" si="1"/>
         <v>0.15618521078092606</v>
       </c>
       <c r="M121">
@@ -6102,7 +6165,7 @@
         <v>0.89800000000000002</v>
       </c>
       <c r="K122">
-        <f>I122/G122</f>
+        <f t="shared" si="1"/>
         <v>0.20293785310734463</v>
       </c>
       <c r="M122">
@@ -6138,7 +6201,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="K123">
-        <f>I123/G123</f>
+        <f t="shared" si="1"/>
         <v>0.36999999999999994</v>
       </c>
       <c r="M123">
@@ -6177,7 +6240,7 @@
         <v>207</v>
       </c>
       <c r="K124">
-        <f>I124/G124</f>
+        <f t="shared" si="1"/>
         <v>0.24628635626014234</v>
       </c>
       <c r="M124">
@@ -6213,7 +6276,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="K125">
-        <f>I125/G125</f>
+        <f t="shared" si="1"/>
         <v>0.3428571428571428</v>
       </c>
       <c r="M125">
@@ -6249,7 +6312,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="K126">
-        <f>I126/G126</f>
+        <f t="shared" si="1"/>
         <v>0.3146067415730337</v>
       </c>
       <c r="M126">
@@ -6285,7 +6348,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K127">
-        <f>I127/G127</f>
+        <f t="shared" si="1"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="M127">
@@ -6321,7 +6384,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K128">
-        <f>I128/G128</f>
+        <f t="shared" si="1"/>
         <v>0.27916666666666667</v>
       </c>
       <c r="M128">
@@ -6357,7 +6420,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="K129">
-        <f>I129/G129</f>
+        <f t="shared" si="1"/>
         <v>0.25405405405405407</v>
       </c>
       <c r="M129">
@@ -6393,7 +6456,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K130">
-        <f>I130/G130</f>
+        <f t="shared" ref="K130:K193" si="2">I130/G130</f>
         <v>0.29545454545454541</v>
       </c>
       <c r="M130">
@@ -6429,7 +6492,7 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="K131">
-        <f>I131/G131</f>
+        <f t="shared" si="2"/>
         <v>0.20935861234368697</v>
       </c>
       <c r="M131">
@@ -6465,7 +6528,7 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="K132">
-        <f>I132/G132</f>
+        <f t="shared" si="2"/>
         <v>0.2050805452292441</v>
       </c>
       <c r="M132">
@@ -6501,7 +6564,7 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="K133">
-        <f>I133/G133</f>
+        <f t="shared" si="2"/>
         <v>0.16473551637279596</v>
       </c>
       <c r="M133">
@@ -6537,7 +6600,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="K134">
-        <f>I134/G134</f>
+        <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
       <c r="M134">
@@ -6573,7 +6636,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="K135">
-        <f>I135/G135</f>
+        <f t="shared" si="2"/>
         <v>0.29870129870129869</v>
       </c>
       <c r="M135">
@@ -6609,7 +6672,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="K136">
-        <f>I136/G136</f>
+        <f t="shared" si="2"/>
         <v>0.28629032258064513</v>
       </c>
       <c r="M136">
@@ -6645,7 +6708,7 @@
         <v>0.39300000000000002</v>
       </c>
       <c r="K137">
-        <f>I137/G137</f>
+        <f t="shared" si="2"/>
         <v>0.4145569620253165</v>
       </c>
       <c r="M137">
@@ -6681,7 +6744,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="K138">
-        <f>I138/G138</f>
+        <f t="shared" si="2"/>
         <v>0.1956368754398311</v>
       </c>
       <c r="M138">
@@ -6717,7 +6780,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K139">
-        <f>I139/G139</f>
+        <f t="shared" si="2"/>
         <v>0.18233082706766918</v>
       </c>
       <c r="M139">
@@ -6753,7 +6816,7 @@
         <v>0.15</v>
       </c>
       <c r="K140">
-        <f>I140/G140</f>
+        <f t="shared" si="2"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="M140">
@@ -6789,7 +6852,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="K141">
-        <f>I141/G141</f>
+        <f t="shared" si="2"/>
         <v>0.20417633410672853</v>
       </c>
       <c r="M141">
@@ -6825,7 +6888,7 @@
         <v>0.108</v>
       </c>
       <c r="K142">
-        <f>I142/G142</f>
+        <f t="shared" si="2"/>
         <v>0.20650095602294455</v>
       </c>
       <c r="M142">
@@ -6861,7 +6924,7 @@
         <v>0.314</v>
       </c>
       <c r="K143">
-        <f>I143/G143</f>
+        <f t="shared" si="2"/>
         <v>0.21820708825573315</v>
       </c>
       <c r="M143">
@@ -6897,7 +6960,7 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="K144">
-        <f>I144/G144</f>
+        <f t="shared" si="2"/>
         <v>0.20233463035019453</v>
       </c>
       <c r="M144">
@@ -6933,7 +6996,7 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="K145">
-        <f>I145/G145</f>
+        <f t="shared" si="2"/>
         <v>0.21382488479262673</v>
       </c>
       <c r="M145">
@@ -6969,7 +7032,7 @@
         <v>0.35899999999999999</v>
       </c>
       <c r="K146">
-        <f>I146/G146</f>
+        <f t="shared" si="2"/>
         <v>0.19638949671772427</v>
       </c>
       <c r="M146">
@@ -7005,7 +7068,7 @@
         <v>0.54</v>
       </c>
       <c r="K147">
-        <f>I147/G147</f>
+        <f t="shared" si="2"/>
         <v>0.21827000808407437</v>
       </c>
       <c r="M147">
@@ -7041,7 +7104,7 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="K148">
-        <f>I148/G148</f>
+        <f t="shared" si="2"/>
         <v>0.19671132764920829</v>
       </c>
       <c r="M148">
@@ -7077,7 +7140,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="K149">
-        <f>I149/G149</f>
+        <f t="shared" si="2"/>
         <v>0.17678868552412647</v>
       </c>
       <c r="M149">
@@ -7113,7 +7176,7 @@
         <v>0.49399999999999999</v>
       </c>
       <c r="K150">
-        <f>I150/G150</f>
+        <f t="shared" si="2"/>
         <v>0.17333333333333334</v>
       </c>
       <c r="M150">
@@ -7149,7 +7212,7 @@
         <v>0.188</v>
       </c>
       <c r="K151">
-        <f>I151/G151</f>
+        <f t="shared" si="2"/>
         <v>0.19282051282051282</v>
       </c>
       <c r="M151">
@@ -7185,7 +7248,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K152">
-        <f>I152/G152</f>
+        <f t="shared" si="2"/>
         <v>0.18210459987397604</v>
       </c>
       <c r="M152">
@@ -7221,7 +7284,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="K153">
-        <f>I153/G153</f>
+        <f t="shared" si="2"/>
         <v>0.18114406779661019</v>
       </c>
       <c r="M153">
@@ -7257,7 +7320,7 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="K154">
-        <f>I154/G154</f>
+        <f t="shared" si="2"/>
         <v>9.9956350938454827E-2</v>
       </c>
       <c r="M154">
@@ -7296,7 +7359,7 @@
         <v>257</v>
       </c>
       <c r="K155">
-        <f>I155/G155</f>
+        <f t="shared" si="2"/>
         <v>0.10982286634460547</v>
       </c>
       <c r="M155">
@@ -7335,7 +7398,7 @@
         <v>259</v>
       </c>
       <c r="K156">
-        <f>I156/G156</f>
+        <f t="shared" si="2"/>
         <v>0.10955686065136146</v>
       </c>
       <c r="M156">
@@ -7371,7 +7434,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="K157">
-        <f>I157/G157</f>
+        <f t="shared" si="2"/>
         <v>0.10804911323328786</v>
       </c>
       <c r="M157">
@@ -7410,7 +7473,7 @@
         <v>262</v>
       </c>
       <c r="K158">
-        <f>I158/G158</f>
+        <f t="shared" si="2"/>
         <v>0.10712166172106824</v>
       </c>
       <c r="M158">
@@ -7446,7 +7509,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="K159">
-        <f>I159/G159</f>
+        <f t="shared" si="2"/>
         <v>0.15313653136531366</v>
       </c>
       <c r="M159">
@@ -7482,7 +7545,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="K160">
-        <f>I160/G160</f>
+        <f t="shared" si="2"/>
         <v>0.16421052631578947</v>
       </c>
       <c r="M160">
@@ -7518,7 +7581,7 @@
         <v>0.05</v>
       </c>
       <c r="K161">
-        <f>I161/G161</f>
+        <f t="shared" si="2"/>
         <v>0.15060240963855423</v>
       </c>
       <c r="M161">
@@ -7554,7 +7617,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="K162">
-        <f>I162/G162</f>
+        <f t="shared" si="2"/>
         <v>0.13989637305699482</v>
       </c>
       <c r="M162">
@@ -7590,7 +7653,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K163">
-        <f>I163/G163</f>
+        <f t="shared" si="2"/>
         <v>0.13483146067415727</v>
       </c>
       <c r="M163">
@@ -7626,7 +7689,7 @@
         <v>0.36399999999999999</v>
       </c>
       <c r="K164">
-        <f>I164/G164</f>
+        <f t="shared" si="2"/>
         <v>0.20289855072463767</v>
       </c>
       <c r="M164">
@@ -7662,7 +7725,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="K165">
-        <f>I165/G165</f>
+        <f t="shared" si="2"/>
         <v>0.14890282131661442</v>
       </c>
       <c r="M165">
@@ -7698,7 +7761,7 @@
         <v>0.11</v>
       </c>
       <c r="K166">
-        <f>I166/G166</f>
+        <f t="shared" si="2"/>
         <v>0.13253012048192772</v>
       </c>
       <c r="M166">
@@ -7734,7 +7797,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K167">
-        <f>I167/G167</f>
+        <f t="shared" si="2"/>
         <v>0.1296625222024867</v>
       </c>
       <c r="M167">
@@ -7770,7 +7833,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="K168">
-        <f>I168/G168</f>
+        <f t="shared" si="2"/>
         <v>0.18580645161290321</v>
       </c>
       <c r="M168">
@@ -7806,7 +7869,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="K169">
-        <f>I169/G169</f>
+        <f t="shared" si="2"/>
         <v>0.19367909238249595</v>
       </c>
       <c r="M169">
@@ -7842,7 +7905,7 @@
         <v>0.153</v>
       </c>
       <c r="K170">
-        <f>I170/G170</f>
+        <f t="shared" si="2"/>
         <v>0.18635809987819732</v>
       </c>
       <c r="M170">
@@ -7878,7 +7941,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="K171">
-        <f>I171/G171</f>
+        <f t="shared" si="2"/>
         <v>0.18611987381703471</v>
       </c>
       <c r="M171">
@@ -7914,7 +7977,7 @@
         <v>0.25</v>
       </c>
       <c r="K172">
-        <f>I172/G172</f>
+        <f t="shared" si="2"/>
         <v>0.19762845849802374</v>
       </c>
       <c r="M172">
@@ -7950,7 +8013,7 @@
         <v>0.84799999999999998</v>
       </c>
       <c r="K173">
-        <f>I173/G173</f>
+        <f t="shared" si="2"/>
         <v>6.8260484585043871E-2</v>
       </c>
       <c r="M173">
@@ -7986,7 +8049,7 @@
         <v>1.036</v>
       </c>
       <c r="K174">
-        <f>I174/G174</f>
+        <f t="shared" si="2"/>
         <v>7.7353841559023376E-2</v>
       </c>
       <c r="M174">
@@ -8022,7 +8085,7 @@
         <v>0.42599999999999999</v>
       </c>
       <c r="K175">
-        <f>I175/G175</f>
+        <f t="shared" si="2"/>
         <v>9.1731266149870802E-2</v>
       </c>
       <c r="M175">
@@ -8058,7 +8121,7 @@
         <v>0.60499999999999998</v>
       </c>
       <c r="K176">
-        <f>I176/G176</f>
+        <f t="shared" si="2"/>
         <v>8.5355530474040625E-2</v>
       </c>
       <c r="M176">
@@ -8094,7 +8157,7 @@
         <v>0.63</v>
       </c>
       <c r="K177">
-        <f>I177/G177</f>
+        <f t="shared" si="2"/>
         <v>7.6754385964912283E-2</v>
       </c>
       <c r="M177">
@@ -8130,7 +8193,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="K178">
-        <f>I178/G178</f>
+        <f t="shared" si="2"/>
         <v>0.24358974358974358</v>
       </c>
       <c r="M178">
@@ -8166,7 +8229,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K179">
-        <f>I179/G179</f>
+        <f t="shared" si="2"/>
         <v>0.23076923076923075</v>
       </c>
       <c r="M179">
@@ -8202,7 +8265,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="K180">
-        <f>I180/G180</f>
+        <f t="shared" si="2"/>
         <v>0.210412147505423</v>
       </c>
       <c r="M180">
@@ -8238,7 +8301,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K181">
-        <f>I181/G181</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="M181">
@@ -8274,7 +8337,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="K182">
-        <f>I182/G182</f>
+        <f t="shared" si="2"/>
         <v>0.19375000000000001</v>
       </c>
       <c r="M182">
@@ -8310,7 +8373,7 @@
         <v>0.127</v>
       </c>
       <c r="K183">
-        <f>I183/G183</f>
+        <f t="shared" si="2"/>
         <v>0.22678571428571426</v>
       </c>
       <c r="M183">
@@ -8346,7 +8409,7 @@
         <v>0.158</v>
       </c>
       <c r="K184">
-        <f>I184/G184</f>
+        <f t="shared" si="2"/>
         <v>0.22067039106145253</v>
       </c>
       <c r="M184">
@@ -8382,7 +8445,7 @@
         <v>0.159</v>
       </c>
       <c r="K185">
-        <f>I185/G185</f>
+        <f t="shared" si="2"/>
         <v>0.24164133738601823</v>
       </c>
       <c r="M185">
@@ -8418,7 +8481,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="K186">
-        <f>I186/G186</f>
+        <f t="shared" si="2"/>
         <v>0.21549421193232413</v>
       </c>
       <c r="M186">
@@ -8454,7 +8517,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="K187">
-        <f>I187/G187</f>
+        <f t="shared" si="2"/>
         <v>0.15271493212669685</v>
       </c>
       <c r="M187">
@@ -8490,7 +8553,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="K188">
-        <f>I188/G188</f>
+        <f t="shared" si="2"/>
         <v>0.15111111111111111</v>
       </c>
       <c r="M188">
@@ -8526,7 +8589,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="K189">
-        <f>I189/G189</f>
+        <f t="shared" si="2"/>
         <v>0.13688212927756652</v>
       </c>
       <c r="M189">
@@ -8562,7 +8625,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="K190">
-        <f>I190/G190</f>
+        <f t="shared" si="2"/>
         <v>0.15837104072398189</v>
       </c>
       <c r="M190">
@@ -8598,7 +8661,7 @@
         <v>0.112</v>
       </c>
       <c r="K191">
-        <f>I191/G191</f>
+        <f t="shared" si="2"/>
         <v>0.13559322033898305</v>
       </c>
       <c r="M191">
@@ -8634,7 +8697,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K192">
-        <f>I192/G192</f>
+        <f t="shared" si="2"/>
         <v>0.12324492979719189</v>
       </c>
       <c r="M192">
@@ -8670,7 +8733,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="K193">
-        <f>I193/G193</f>
+        <f t="shared" si="2"/>
         <v>0.16300940438871472</v>
       </c>
       <c r="M193">
@@ -8706,7 +8769,7 @@
         <v>0.124</v>
       </c>
       <c r="K194">
-        <f>I194/G194</f>
+        <f t="shared" ref="K194:K257" si="3">I194/G194</f>
         <v>0.15066828675577157</v>
       </c>
       <c r="M194">
@@ -8742,7 +8805,7 @@
         <v>0.113</v>
       </c>
       <c r="K195">
-        <f>I195/G195</f>
+        <f t="shared" si="3"/>
         <v>0.13647342995169084</v>
       </c>
       <c r="M195">
@@ -8778,7 +8841,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="K196">
-        <f>I196/G196</f>
+        <f t="shared" si="3"/>
         <v>0.17346938775510204</v>
       </c>
       <c r="M196">
@@ -8814,7 +8877,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="K197">
-        <f>I197/G197</f>
+        <f t="shared" si="3"/>
         <v>0.17375886524822695</v>
       </c>
       <c r="M197">
@@ -8850,7 +8913,7 @@
         <v>0.03</v>
       </c>
       <c r="K198">
-        <f>I198/G198</f>
+        <f t="shared" si="3"/>
         <v>0.19480519480519479</v>
       </c>
       <c r="M198">
@@ -8886,7 +8949,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="K199">
-        <f>I199/G199</f>
+        <f t="shared" si="3"/>
         <v>0.178343949044586</v>
       </c>
       <c r="M199">
@@ -8922,7 +8985,7 @@
         <v>0.217</v>
       </c>
       <c r="K200">
-        <f>I200/G200</f>
+        <f t="shared" si="3"/>
         <v>0.16476841305998483</v>
       </c>
       <c r="M200">
@@ -8958,7 +9021,7 @@
         <v>0.14899999999999999</v>
       </c>
       <c r="K201">
-        <f>I201/G201</f>
+        <f t="shared" si="3"/>
         <v>0.14272030651340994</v>
       </c>
       <c r="M201">
@@ -8994,7 +9057,7 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="K202">
-        <f>I202/G202</f>
+        <f t="shared" si="3"/>
         <v>0.15776699029126215</v>
       </c>
       <c r="M202">
@@ -9030,7 +9093,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="K203">
-        <f>I203/G203</f>
+        <f t="shared" si="3"/>
         <v>0.12428842504743833</v>
       </c>
       <c r="M203">
@@ -9066,7 +9129,7 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="K204">
-        <f>I204/G204</f>
+        <f t="shared" si="3"/>
         <v>0.13804971319311662</v>
       </c>
       <c r="M204">
@@ -9102,7 +9165,7 @@
         <v>0.189</v>
       </c>
       <c r="K205">
-        <f>I205/G205</f>
+        <f t="shared" si="3"/>
         <v>0.13815789473684209</v>
       </c>
       <c r="M205">
@@ -9138,7 +9201,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="K206">
-        <f>I206/G206</f>
+        <f t="shared" si="3"/>
         <v>0.1411822178798241</v>
       </c>
       <c r="M206">
@@ -9174,7 +9237,7 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="K207">
-        <f>I207/G207</f>
+        <f t="shared" si="3"/>
         <v>0.12414042707202318</v>
       </c>
       <c r="M207">
@@ -9210,7 +9273,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="K208">
-        <f>I208/G208</f>
+        <f t="shared" si="3"/>
         <v>0.13170272812793982</v>
       </c>
       <c r="M208">
@@ -9246,7 +9309,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="K209">
-        <f>I209/G209</f>
+        <f t="shared" si="3"/>
         <v>0.12742812742812745</v>
       </c>
       <c r="M209">
@@ -9282,7 +9345,7 @@
         <v>0.12</v>
       </c>
       <c r="K210">
-        <f>I210/G210</f>
+        <f t="shared" si="3"/>
         <v>0.19108280254777069</v>
       </c>
       <c r="M210">
@@ -9318,7 +9381,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="K211">
-        <f>I211/G211</f>
+        <f t="shared" si="3"/>
         <v>0.20435967302452315</v>
       </c>
       <c r="M211">
@@ -9354,7 +9417,7 @@
         <v>0.05</v>
       </c>
       <c r="K212">
-        <f>I212/G212</f>
+        <f t="shared" si="3"/>
         <v>0.2183406113537118</v>
       </c>
       <c r="M212">
@@ -9393,7 +9456,7 @@
         <v>329</v>
       </c>
       <c r="K213">
-        <f>I213/G213</f>
+        <f t="shared" si="3"/>
         <v>0.12863436123348018</v>
       </c>
       <c r="M213">
@@ -9429,7 +9492,7 @@
         <v>0.69499999999999995</v>
       </c>
       <c r="K214">
-        <f>I214/G214</f>
+        <f t="shared" si="3"/>
         <v>0.11831801157643854</v>
       </c>
       <c r="M214">
@@ -9468,7 +9531,7 @@
         <v>332</v>
       </c>
       <c r="K215">
-        <f>I215/G215</f>
+        <f t="shared" si="3"/>
         <v>0.12973508294132211</v>
       </c>
       <c r="M215">
@@ -9504,7 +9567,7 @@
         <v>0.53300000000000003</v>
       </c>
       <c r="K216">
-        <f>I216/G216</f>
+        <f t="shared" si="3"/>
         <v>0.11162303664921466</v>
       </c>
       <c r="M216">
@@ -9540,7 +9603,7 @@
         <v>0.66900000000000004</v>
       </c>
       <c r="K217">
-        <f>I217/G217</f>
+        <f t="shared" si="3"/>
         <v>7.5253093363329582E-2</v>
       </c>
       <c r="M217">
@@ -9576,7 +9639,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K218">
-        <f>I218/G218</f>
+        <f t="shared" si="3"/>
         <v>0.26315789473684209</v>
       </c>
       <c r="M218">
@@ -9612,7 +9675,7 @@
         <v>0.128</v>
       </c>
       <c r="K219">
-        <f>I219/G219</f>
+        <f t="shared" si="3"/>
         <v>0.24854368932038834</v>
       </c>
       <c r="M219">
@@ -9648,7 +9711,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="K220">
-        <f>I220/G220</f>
+        <f t="shared" si="3"/>
         <v>0.24781341107871721</v>
       </c>
       <c r="M220">
@@ -9684,7 +9747,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="K221">
-        <f>I221/G221</f>
+        <f t="shared" si="3"/>
         <v>0.23268698060941831</v>
       </c>
       <c r="M221">
@@ -9720,7 +9783,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="K222">
-        <f>I222/G222</f>
+        <f t="shared" si="3"/>
         <v>0.23719676549865229</v>
       </c>
       <c r="M222">
@@ -9756,7 +9819,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="K223">
-        <f>I223/G223</f>
+        <f t="shared" si="3"/>
         <v>0.25454545454545457</v>
       </c>
       <c r="M223">
@@ -9792,7 +9855,7 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="K224">
-        <f>I224/G224</f>
+        <f t="shared" si="3"/>
         <v>0.23529411764705885</v>
       </c>
       <c r="M224">
@@ -9828,7 +9891,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="K225">
-        <f>I225/G225</f>
+        <f t="shared" si="3"/>
         <v>0.24277456647398848</v>
       </c>
       <c r="M225">
@@ -9864,7 +9927,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="K226">
-        <f>I226/G226</f>
+        <f t="shared" si="3"/>
         <v>0.27492447129909364</v>
       </c>
       <c r="M226">
@@ -9900,7 +9963,7 @@
         <v>0.1</v>
       </c>
       <c r="K227">
-        <f>I227/G227</f>
+        <f t="shared" si="3"/>
         <v>0.24330900243309006</v>
       </c>
       <c r="M227">
@@ -9936,7 +9999,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="K228">
-        <f>I228/G228</f>
+        <f t="shared" si="3"/>
         <v>0.1669921875</v>
       </c>
       <c r="M228">
@@ -9972,7 +10035,7 @@
         <v>0.23499999999999999</v>
       </c>
       <c r="K229">
-        <f>I229/G229</f>
+        <f t="shared" si="3"/>
         <v>0.15793010752688172</v>
       </c>
       <c r="M229">
@@ -10008,7 +10071,7 @@
         <v>0.20899999999999999</v>
       </c>
       <c r="K230">
-        <f>I230/G230</f>
+        <f t="shared" si="3"/>
         <v>0.15300146412884333</v>
       </c>
       <c r="M230">
@@ -10044,7 +10107,7 @@
         <v>0.124</v>
       </c>
       <c r="K231">
-        <f>I231/G231</f>
+        <f t="shared" si="3"/>
         <v>0.16916780354706684</v>
       </c>
       <c r="M231">
@@ -10080,7 +10143,7 @@
         <v>0.121</v>
       </c>
       <c r="K232">
-        <f>I232/G232</f>
+        <f t="shared" si="3"/>
         <v>0.19803600654664485</v>
       </c>
       <c r="M232">
@@ -10116,7 +10179,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="K233">
-        <f>I233/G233</f>
+        <f t="shared" si="3"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="M233">
@@ -10152,7 +10215,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="K234">
-        <f>I234/G234</f>
+        <f t="shared" si="3"/>
         <v>0.26909090909090905</v>
       </c>
       <c r="M234">
@@ -10188,7 +10251,7 @@
         <v>0.18</v>
       </c>
       <c r="K235">
-        <f>I235/G235</f>
+        <f t="shared" si="3"/>
         <v>0.20134228187919462</v>
       </c>
       <c r="M235">
@@ -10224,7 +10287,7 @@
         <v>0.223</v>
       </c>
       <c r="K236">
-        <f>I236/G236</f>
+        <f t="shared" si="3"/>
         <v>0.22211155378486055</v>
       </c>
       <c r="M236">
@@ -10260,7 +10323,7 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="K237">
-        <f>I237/G237</f>
+        <f t="shared" si="3"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="M237">
@@ -10296,7 +10359,7 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="K238">
-        <f>I238/G238</f>
+        <f t="shared" si="3"/>
         <v>0.18285065303804657</v>
       </c>
       <c r="M238">
@@ -10332,7 +10395,7 @@
         <v>0.34599999999999997</v>
       </c>
       <c r="K239">
-        <f>I239/G239</f>
+        <f t="shared" si="3"/>
         <v>0.20364920541494994</v>
       </c>
       <c r="M239">
@@ -10368,7 +10431,7 @@
         <v>0.307</v>
       </c>
       <c r="K240">
-        <f>I240/G240</f>
+        <f t="shared" si="3"/>
         <v>0.20398671096345516</v>
       </c>
       <c r="M240">
@@ -10404,7 +10467,7 @@
         <v>0.253</v>
       </c>
       <c r="K241">
-        <f>I241/G241</f>
+        <f t="shared" si="3"/>
         <v>0.20891824938067713</v>
       </c>
       <c r="M241">
@@ -10440,7 +10503,7 @@
         <v>0.126</v>
       </c>
       <c r="K242">
-        <f>I242/G242</f>
+        <f t="shared" si="3"/>
         <v>0.2475442043222004</v>
       </c>
       <c r="M242">
@@ -10476,7 +10539,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="K243">
-        <f>I243/G243</f>
+        <f t="shared" si="3"/>
         <v>0.22105263157894739</v>
       </c>
       <c r="M243">
@@ -10512,7 +10575,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="K244">
-        <f>I244/G244</f>
+        <f t="shared" si="3"/>
         <v>0.22564102564102562</v>
       </c>
       <c r="M244">
@@ -10548,7 +10611,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="K245">
-        <f>I245/G245</f>
+        <f t="shared" si="3"/>
         <v>0.19881305637982197</v>
       </c>
       <c r="M245">
@@ -10584,7 +10647,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="K246">
-        <f>I246/G246</f>
+        <f t="shared" si="3"/>
         <v>0.2282051282051282</v>
       </c>
       <c r="M246">
@@ -10620,7 +10683,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="K247">
-        <f>I247/G247</f>
+        <f t="shared" si="3"/>
         <v>0.21637426900584791</v>
       </c>
       <c r="M247">
@@ -10656,7 +10719,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K248">
-        <f>I248/G248</f>
+        <f t="shared" si="3"/>
         <v>0.25280898876404495</v>
       </c>
       <c r="M248">
@@ -10692,7 +10755,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="K249">
-        <f>I249/G249</f>
+        <f t="shared" si="3"/>
         <v>0.19148936170212766</v>
       </c>
       <c r="M249">
@@ -10728,7 +10791,7 @@
         <v>0.126</v>
       </c>
       <c r="K250">
-        <f>I250/G250</f>
+        <f t="shared" si="3"/>
         <v>0.20487804878048782</v>
       </c>
       <c r="M250">
@@ -10764,7 +10827,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="K251">
-        <f>I251/G251</f>
+        <f t="shared" si="3"/>
         <v>0.21662468513853902</v>
       </c>
       <c r="M251">
@@ -10800,7 +10863,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="K252">
-        <f>I252/G252</f>
+        <f t="shared" si="3"/>
         <v>0.27327935222672067</v>
       </c>
       <c r="M252">
@@ -10836,7 +10899,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="K253">
-        <f>I253/G253</f>
+        <f t="shared" si="3"/>
         <v>0.26427406199021208</v>
       </c>
       <c r="M253">
@@ -10872,7 +10935,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="K254">
-        <f>I254/G254</f>
+        <f t="shared" si="3"/>
         <v>0.25268817204301069</v>
       </c>
       <c r="M254">
@@ -10908,7 +10971,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="K255">
-        <f>I255/G255</f>
+        <f t="shared" si="3"/>
         <v>0.25192012288786481</v>
       </c>
       <c r="M255">
@@ -10944,7 +11007,7 @@
         <v>0.107</v>
       </c>
       <c r="K256">
-        <f>I256/G256</f>
+        <f t="shared" si="3"/>
         <v>0.28232189973614774</v>
       </c>
       <c r="M256">
@@ -10980,7 +11043,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="K257">
-        <f>I257/G257</f>
+        <f t="shared" si="3"/>
         <v>0.25874125874125875</v>
       </c>
       <c r="M257">
@@ -11016,7 +11079,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="K258">
-        <f>I258/G258</f>
+        <f t="shared" ref="K258:K308" si="4">I258/G258</f>
         <v>0.2087591240875912</v>
       </c>
       <c r="M258">
@@ -11052,7 +11115,7 @@
         <v>0.185</v>
       </c>
       <c r="K259">
-        <f>I259/G259</f>
+        <f t="shared" si="4"/>
         <v>0.27903469079939669</v>
       </c>
       <c r="M259">
@@ -11088,7 +11151,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="K260">
-        <f>I260/G260</f>
+        <f t="shared" si="4"/>
         <v>0.32334384858044163</v>
       </c>
       <c r="M260">
@@ -11124,7 +11187,7 @@
         <v>0.246</v>
       </c>
       <c r="K261">
-        <f>I261/G261</f>
+        <f t="shared" si="4"/>
         <v>0.27003293084522501</v>
       </c>
       <c r="M261">
@@ -11160,7 +11223,7 @@
         <v>0.39400000000000002</v>
       </c>
       <c r="K262">
-        <f>I262/G262</f>
+        <f t="shared" si="4"/>
         <v>0.13007593265103995</v>
       </c>
       <c r="M262">
@@ -11196,7 +11259,7 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="K263">
-        <f>I263/G263</f>
+        <f t="shared" si="4"/>
         <v>0.11967779056386652</v>
       </c>
       <c r="M263">
@@ -11232,7 +11295,7 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="K264">
-        <f>I264/G264</f>
+        <f t="shared" si="4"/>
         <v>0.13796716730702061</v>
       </c>
       <c r="M264">
@@ -11268,7 +11331,7 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="K265">
-        <f>I265/G265</f>
+        <f t="shared" si="4"/>
         <v>0.12688049957422651</v>
       </c>
       <c r="M265">
@@ -11307,7 +11370,7 @@
         <v>395</v>
       </c>
       <c r="K266">
-        <f>I266/G266</f>
+        <f t="shared" si="4"/>
         <v>0.10710301227222015</v>
       </c>
       <c r="M266">
@@ -11343,7 +11406,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="K267">
-        <f>I267/G267</f>
+        <f t="shared" si="4"/>
         <v>0.17938144329896907</v>
       </c>
       <c r="M267">
@@ -11379,7 +11442,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="K268">
-        <f>I268/G268</f>
+        <f t="shared" si="4"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="M268">
@@ -11415,7 +11478,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="K269">
-        <f>I269/G269</f>
+        <f t="shared" si="4"/>
         <v>0.18497109826589597</v>
       </c>
       <c r="M269">
@@ -11451,7 +11514,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="K270">
-        <f>I270/G270</f>
+        <f t="shared" si="4"/>
         <v>0.18067226890756302</v>
       </c>
       <c r="M270">
@@ -11487,7 +11550,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="K271">
-        <f>I271/G271</f>
+        <f t="shared" si="4"/>
         <v>0.15533980582524273</v>
       </c>
       <c r="M271">
@@ -11523,7 +11586,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="K272">
-        <f>I272/G272</f>
+        <f t="shared" si="4"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="M272">
@@ -11559,7 +11622,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="K273">
-        <f>I273/G273</f>
+        <f t="shared" si="4"/>
         <v>0.16804407713498623</v>
       </c>
       <c r="M273">
@@ -11595,7 +11658,7 @@
         <v>0.33</v>
       </c>
       <c r="K274">
-        <f>I274/G274</f>
+        <f t="shared" si="4"/>
         <v>0.13819095477386936</v>
       </c>
       <c r="M274">
@@ -11631,7 +11694,7 @@
         <v>0.20899999999999999</v>
       </c>
       <c r="K275">
-        <f>I275/G275</f>
+        <f t="shared" si="4"/>
         <v>0.13062499999999999</v>
       </c>
       <c r="M275">
@@ -11667,7 +11730,7 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="K276">
-        <f>I276/G276</f>
+        <f t="shared" si="4"/>
         <v>0.12740384615384615</v>
       </c>
       <c r="M276">
@@ -11703,7 +11766,7 @@
         <v>0.56599999999999995</v>
       </c>
       <c r="K277">
-        <f>I277/G277</f>
+        <f t="shared" si="4"/>
         <v>0.12466960352422907</v>
       </c>
       <c r="M277">
@@ -11742,7 +11805,7 @@
         <v>410</v>
       </c>
       <c r="K278">
-        <f>I278/G278</f>
+        <f t="shared" si="4"/>
         <v>0.13351375732972487</v>
       </c>
       <c r="M278">
@@ -11778,7 +11841,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="K279">
-        <f>I279/G279</f>
+        <f t="shared" si="4"/>
         <v>0.23753665689149558</v>
       </c>
       <c r="M279">
@@ -11814,7 +11877,7 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="K280">
-        <f>I280/G280</f>
+        <f t="shared" si="4"/>
         <v>0.2213225371120108</v>
       </c>
       <c r="M280">
@@ -11850,7 +11913,7 @@
         <v>0.156</v>
       </c>
       <c r="K281">
-        <f>I281/G281</f>
+        <f t="shared" si="4"/>
         <v>0.22096317280453259</v>
       </c>
       <c r="M281">
@@ -11886,7 +11949,7 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="K282">
-        <f>I282/G282</f>
+        <f t="shared" si="4"/>
         <v>0.23042647994907703</v>
       </c>
       <c r="M282">
@@ -11922,7 +11985,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="K283">
-        <f>I283/G283</f>
+        <f t="shared" si="4"/>
         <v>0.36538461538461542</v>
       </c>
       <c r="M283">
@@ -11958,7 +12021,7 @@
         <v>0.124</v>
       </c>
       <c r="K284">
-        <f>I284/G284</f>
+        <f t="shared" si="4"/>
         <v>0.33787465940054495</v>
       </c>
       <c r="M284">
@@ -11994,7 +12057,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="K285">
-        <f>I285/G285</f>
+        <f t="shared" si="4"/>
         <v>0.29531568228105903</v>
       </c>
       <c r="M285">
@@ -12030,7 +12093,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K286">
-        <f>I286/G286</f>
+        <f t="shared" si="4"/>
         <v>0.28937728937728935</v>
       </c>
       <c r="M286">
@@ -12066,7 +12129,7 @@
         <v>0.373</v>
       </c>
       <c r="K287">
-        <f>I287/G287</f>
+        <f t="shared" si="4"/>
         <v>0.26138752627890677</v>
       </c>
       <c r="M287">
@@ -12102,7 +12165,7 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="K288">
-        <f>I288/G288</f>
+        <f t="shared" si="4"/>
         <v>0.3378076062639821</v>
       </c>
       <c r="M288">
@@ -12138,7 +12201,7 @@
         <v>0.17</v>
       </c>
       <c r="K289">
-        <f>I289/G289</f>
+        <f t="shared" si="4"/>
         <v>0.24566473988439311</v>
       </c>
       <c r="M289">
@@ -12174,7 +12237,7 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="K290">
-        <f>I290/G290</f>
+        <f t="shared" si="4"/>
         <v>0.23868312757201648</v>
       </c>
       <c r="M290">
@@ -12210,11 +12273,623 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="K291">
-        <f>I291/G291</f>
+        <f t="shared" si="4"/>
         <v>0.32949308755760365</v>
       </c>
       <c r="M291">
         <v>4</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>86</v>
+      </c>
+      <c r="B292" t="s">
+        <v>427</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D292" t="s">
+        <v>429</v>
+      </c>
+      <c r="E292">
+        <v>1</v>
+      </c>
+      <c r="F292">
+        <v>3</v>
+      </c>
+      <c r="G292">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H292" t="s">
+        <v>430</v>
+      </c>
+      <c r="I292">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="K292">
+        <f t="shared" si="4"/>
+        <v>0.26829268292682923</v>
+      </c>
+      <c r="M292">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>86</v>
+      </c>
+      <c r="B293" t="s">
+        <v>427</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D293" t="s">
+        <v>429</v>
+      </c>
+      <c r="E293">
+        <v>2</v>
+      </c>
+      <c r="F293">
+        <v>4</v>
+      </c>
+      <c r="G293">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="H293" t="s">
+        <v>431</v>
+      </c>
+      <c r="I293">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K293">
+        <f t="shared" si="4"/>
+        <v>0.27731092436974791</v>
+      </c>
+      <c r="M293">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>86</v>
+      </c>
+      <c r="B294" t="s">
+        <v>427</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D294" t="s">
+        <v>429</v>
+      </c>
+      <c r="E294">
+        <v>3</v>
+      </c>
+      <c r="F294">
+        <v>4</v>
+      </c>
+      <c r="G294">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="H294" t="s">
+        <v>432</v>
+      </c>
+      <c r="I294">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K294">
+        <f t="shared" si="4"/>
+        <v>0.28895184135977336</v>
+      </c>
+      <c r="M294">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>86</v>
+      </c>
+      <c r="B295" t="s">
+        <v>427</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D295" t="s">
+        <v>429</v>
+      </c>
+      <c r="E295">
+        <v>4</v>
+      </c>
+      <c r="F295">
+        <v>4</v>
+      </c>
+      <c r="G295">
+        <v>0.497</v>
+      </c>
+      <c r="H295" t="s">
+        <v>433</v>
+      </c>
+      <c r="I295">
+        <v>0.125</v>
+      </c>
+      <c r="K295">
+        <f t="shared" si="4"/>
+        <v>0.25150905432595572</v>
+      </c>
+      <c r="M295">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>86</v>
+      </c>
+      <c r="B296" t="s">
+        <v>427</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D296" t="s">
+        <v>429</v>
+      </c>
+      <c r="E296">
+        <v>5</v>
+      </c>
+      <c r="F296">
+        <v>4</v>
+      </c>
+      <c r="G296">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="H296" t="s">
+        <v>434</v>
+      </c>
+      <c r="I296">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K296">
+        <f t="shared" si="4"/>
+        <v>0.22525597269624575</v>
+      </c>
+      <c r="M296">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>86</v>
+      </c>
+      <c r="B297" t="s">
+        <v>427</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D297" t="s">
+        <v>429</v>
+      </c>
+      <c r="E297">
+        <v>6</v>
+      </c>
+      <c r="F297">
+        <v>4</v>
+      </c>
+      <c r="G297">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H297" t="s">
+        <v>435</v>
+      </c>
+      <c r="I297">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K297">
+        <f t="shared" si="4"/>
+        <v>0.27485380116959063</v>
+      </c>
+      <c r="M297">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>86</v>
+      </c>
+      <c r="B298" t="s">
+        <v>427</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D298" t="s">
+        <v>429</v>
+      </c>
+      <c r="E298">
+        <v>7</v>
+      </c>
+      <c r="F298">
+        <v>4</v>
+      </c>
+      <c r="G298">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="H298" t="s">
+        <v>436</v>
+      </c>
+      <c r="I298">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K298">
+        <f t="shared" si="4"/>
+        <v>0.26394052044609662</v>
+      </c>
+      <c r="M298">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>86</v>
+      </c>
+      <c r="B299" t="s">
+        <v>427</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D299" t="s">
+        <v>429</v>
+      </c>
+      <c r="E299">
+        <v>8</v>
+      </c>
+      <c r="F299">
+        <v>4</v>
+      </c>
+      <c r="G299">
+        <v>0.307</v>
+      </c>
+      <c r="H299" t="s">
+        <v>437</v>
+      </c>
+      <c r="I299">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="K299">
+        <f t="shared" si="4"/>
+        <v>0.28990228013029318</v>
+      </c>
+      <c r="M299">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>86</v>
+      </c>
+      <c r="B300" t="s">
+        <v>427</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D300" t="s">
+        <v>429</v>
+      </c>
+      <c r="E300">
+        <v>9</v>
+      </c>
+      <c r="F300">
+        <v>3</v>
+      </c>
+      <c r="G300">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="H300" t="s">
+        <v>438</v>
+      </c>
+      <c r="I300">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K300">
+        <f t="shared" si="4"/>
+        <v>0.25352112676056338</v>
+      </c>
+      <c r="M300">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>327</v>
+      </c>
+      <c r="B301" t="s">
+        <v>439</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D301" t="s">
+        <v>429</v>
+      </c>
+      <c r="E301">
+        <v>1</v>
+      </c>
+      <c r="F301">
+        <v>2</v>
+      </c>
+      <c r="G301">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="H301" t="s">
+        <v>440</v>
+      </c>
+      <c r="I301">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K301">
+        <f t="shared" si="4"/>
+        <v>0.13212795549374132</v>
+      </c>
+      <c r="M301">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>327</v>
+      </c>
+      <c r="B302" t="s">
+        <v>439</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D302" t="s">
+        <v>429</v>
+      </c>
+      <c r="E302">
+        <v>2</v>
+      </c>
+      <c r="F302">
+        <v>2</v>
+      </c>
+      <c r="G302">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="H302" t="s">
+        <v>441</v>
+      </c>
+      <c r="I302">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K302">
+        <f t="shared" si="4"/>
+        <v>0.12530712530712532</v>
+      </c>
+      <c r="M302">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>327</v>
+      </c>
+      <c r="B303" t="s">
+        <v>439</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D303" t="s">
+        <v>429</v>
+      </c>
+      <c r="E303">
+        <v>3</v>
+      </c>
+      <c r="F303">
+        <v>3</v>
+      </c>
+      <c r="G303">
+        <v>1.151</v>
+      </c>
+      <c r="H303" t="s">
+        <v>442</v>
+      </c>
+      <c r="I303">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="K303">
+        <f t="shared" si="4"/>
+        <v>0.11815812337098176</v>
+      </c>
+      <c r="M303">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>327</v>
+      </c>
+      <c r="B304" t="s">
+        <v>439</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D304" t="s">
+        <v>429</v>
+      </c>
+      <c r="E304">
+        <v>4</v>
+      </c>
+      <c r="F304">
+        <v>3</v>
+      </c>
+      <c r="G304">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="H304" t="s">
+        <v>443</v>
+      </c>
+      <c r="I304">
+        <v>9.4E-2</v>
+      </c>
+      <c r="K304">
+        <f t="shared" si="4"/>
+        <v>0.1346704871060172</v>
+      </c>
+      <c r="M304">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>327</v>
+      </c>
+      <c r="B305" t="s">
+        <v>439</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D305" t="s">
+        <v>429</v>
+      </c>
+      <c r="E305">
+        <v>5</v>
+      </c>
+      <c r="F305">
+        <v>2</v>
+      </c>
+      <c r="G305">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="H305" t="s">
+        <v>444</v>
+      </c>
+      <c r="I305">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="K305">
+        <f t="shared" si="4"/>
+        <v>0.12948857453754078</v>
+      </c>
+      <c r="M305">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>327</v>
+      </c>
+      <c r="B306" t="s">
+        <v>439</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D306" t="s">
+        <v>429</v>
+      </c>
+      <c r="E306">
+        <v>6</v>
+      </c>
+      <c r="F306">
+        <v>1</v>
+      </c>
+      <c r="G306">
+        <v>0.311</v>
+      </c>
+      <c r="H306" t="s">
+        <v>445</v>
+      </c>
+      <c r="I306">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K306">
+        <f t="shared" si="4"/>
+        <v>0.10289389067524116</v>
+      </c>
+      <c r="M306">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>327</v>
+      </c>
+      <c r="B307" t="s">
+        <v>439</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D307" t="s">
+        <v>429</v>
+      </c>
+      <c r="E307">
+        <v>7</v>
+      </c>
+      <c r="F307">
+        <v>1</v>
+      </c>
+      <c r="G307">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="H307" t="s">
+        <v>446</v>
+      </c>
+      <c r="I307">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K307">
+        <f t="shared" si="4"/>
+        <v>0.10690423162583519</v>
+      </c>
+      <c r="M307">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>327</v>
+      </c>
+      <c r="B308" t="s">
+        <v>439</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D308" t="s">
+        <v>429</v>
+      </c>
+      <c r="E308">
+        <v>8</v>
+      </c>
+      <c r="F308">
+        <v>2</v>
+      </c>
+      <c r="G308">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="H308" t="s">
+        <v>447</v>
+      </c>
+      <c r="I308">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="K308">
+        <f t="shared" si="4"/>
+        <v>9.6638655462184878E-2</v>
+      </c>
+      <c r="M308">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>